<commit_message>
Recorded pages numbers for book 2.
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415DFFC4-6F7F-3344-B8D9-BAF59DA8650A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE347A8-8E53-1F40-A6A3-1F282A2125D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>Stormlight Achive Book Info</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>End Page</t>
+  </si>
+  <si>
+    <t>Book 2 Chapter Pages (counting from 1)</t>
+  </si>
+  <si>
+    <t>I-10</t>
+  </si>
+  <si>
+    <t>I-11</t>
+  </si>
+  <si>
+    <t>I-12</t>
+  </si>
+  <si>
+    <t>I-13</t>
+  </si>
+  <si>
+    <t>I-14</t>
+  </si>
+  <si>
+    <t>Book 3 Chapter Pages (counting from 1)</t>
   </si>
 </sst>
 </file>
@@ -456,23 +477,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -486,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -500,7 +524,7 @@
         <v>383389</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -514,7 +538,7 @@
         <v>399431</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -528,7 +552,7 @@
         <v>451912</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -542,722 +566,2300 @@
         <v>455891</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>41</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>67</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>86</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>96</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>112</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>155</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="M19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
         <v>132</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>164</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21">
         <v>151</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>174</v>
+      </c>
+      <c r="I21">
+        <v>9</v>
+      </c>
+      <c r="M21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
       <c r="B22">
         <v>173</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>185</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="M22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
       <c r="B23">
         <v>181</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>189</v>
+      </c>
+      <c r="I23">
+        <v>11</v>
+      </c>
+      <c r="M23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
       <c r="B24">
         <v>189</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>203</v>
+      </c>
+      <c r="I24">
+        <v>12</v>
+      </c>
+      <c r="M24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>221</v>
+      </c>
+      <c r="I25">
+        <v>13</v>
+      </c>
+      <c r="M25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26">
         <v>208</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>233</v>
+      </c>
+      <c r="I26">
+        <v>14</v>
+      </c>
+      <c r="M26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27">
         <v>213</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>243</v>
+      </c>
+      <c r="I27">
+        <v>15</v>
+      </c>
+      <c r="M27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
       <c r="B28">
         <v>221</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28">
+        <v>268</v>
+      </c>
+      <c r="I28">
+        <v>16</v>
+      </c>
+      <c r="M28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>13</v>
       </c>
       <c r="B29">
         <v>245</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>13</v>
+      </c>
+      <c r="F29">
+        <v>283</v>
+      </c>
+      <c r="I29">
+        <v>17</v>
+      </c>
+      <c r="M29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30">
         <v>256</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>14</v>
+      </c>
+      <c r="F30">
+        <v>294</v>
+      </c>
+      <c r="I30">
+        <v>18</v>
+      </c>
+      <c r="M30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31">
         <v>268</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>305</v>
+      </c>
+      <c r="I31">
+        <v>19</v>
+      </c>
+      <c r="M31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>
       <c r="B32">
         <v>297</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>313</v>
+      </c>
+      <c r="I32">
+        <v>20</v>
+      </c>
+      <c r="M32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>17</v>
       </c>
       <c r="B33">
         <v>314</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>17</v>
+      </c>
+      <c r="F33">
+        <v>330</v>
+      </c>
+      <c r="I33">
+        <v>21</v>
+      </c>
+      <c r="M33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>18</v>
       </c>
       <c r="B34">
         <v>345</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>18</v>
+      </c>
+      <c r="F34">
+        <v>347</v>
+      </c>
+      <c r="I34">
+        <v>22</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>19</v>
       </c>
       <c r="B35">
         <v>361</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>19</v>
+      </c>
+      <c r="F35">
+        <v>361</v>
+      </c>
+      <c r="I35">
+        <v>23</v>
+      </c>
+      <c r="M35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36">
         <v>379</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>366</v>
+      </c>
+      <c r="I36">
+        <v>24</v>
+      </c>
+      <c r="M36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>21</v>
       </c>
       <c r="B37">
         <v>382</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>21</v>
+      </c>
+      <c r="F37">
+        <v>376</v>
+      </c>
+      <c r="I37">
+        <v>25</v>
+      </c>
+      <c r="M37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>22</v>
       </c>
       <c r="B38">
         <v>396</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>22</v>
+      </c>
+      <c r="F38">
+        <v>386</v>
+      </c>
+      <c r="I38">
+        <v>26</v>
+      </c>
+      <c r="M38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>23</v>
       </c>
       <c r="B39">
         <v>414</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>23</v>
+      </c>
+      <c r="F39">
+        <v>402</v>
+      </c>
+      <c r="I39">
+        <v>27</v>
+      </c>
+      <c r="M39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>24</v>
       </c>
       <c r="B40">
         <v>432</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>24</v>
+      </c>
+      <c r="F40">
+        <v>409</v>
+      </c>
+      <c r="I40">
+        <v>28</v>
+      </c>
+      <c r="M40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>25</v>
       </c>
       <c r="B41">
         <v>444</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>25</v>
+      </c>
+      <c r="F41">
+        <v>424</v>
+      </c>
+      <c r="I41">
+        <v>29</v>
+      </c>
+      <c r="M41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>26</v>
       </c>
       <c r="B42">
         <v>454</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>26</v>
+      </c>
+      <c r="F42">
+        <v>440</v>
+      </c>
+      <c r="I42">
+        <v>30</v>
+      </c>
+      <c r="M42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>27</v>
       </c>
       <c r="B43">
         <v>474</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>27</v>
+      </c>
+      <c r="F43">
+        <v>454</v>
+      </c>
+      <c r="I43">
+        <v>31</v>
+      </c>
+      <c r="M43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>28</v>
       </c>
       <c r="B44">
         <v>501</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>28</v>
+      </c>
+      <c r="F44">
+        <v>458</v>
+      </c>
+      <c r="I44">
+        <v>32</v>
+      </c>
+      <c r="M44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45">
         <v>532</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>29</v>
+      </c>
+      <c r="F45">
+        <v>469</v>
+      </c>
+      <c r="I45" t="s">
+        <v>10</v>
+      </c>
+      <c r="M45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
       <c r="B46">
         <v>541</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>30</v>
+      </c>
+      <c r="F46">
+        <v>481</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="M46">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
       <c r="B47">
         <v>548</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>31</v>
+      </c>
+      <c r="F47">
+        <v>491</v>
+      </c>
+      <c r="I47" t="s">
+        <v>12</v>
+      </c>
+      <c r="M47">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>29</v>
       </c>
       <c r="B48">
         <v>560</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>32</v>
+      </c>
+      <c r="F48">
+        <v>500</v>
+      </c>
+      <c r="I48">
+        <v>33</v>
+      </c>
+      <c r="M48">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>30</v>
       </c>
       <c r="B49">
         <v>581</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>33</v>
+      </c>
+      <c r="F49">
+        <v>513</v>
+      </c>
+      <c r="I49">
+        <v>34</v>
+      </c>
+      <c r="M49">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>31</v>
       </c>
       <c r="B50">
         <v>593</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>34</v>
+      </c>
+      <c r="F50">
+        <v>524</v>
+      </c>
+      <c r="I50">
+        <v>35</v>
+      </c>
+      <c r="M50">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>32</v>
       </c>
       <c r="B51">
         <v>600</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>536</v>
+      </c>
+      <c r="I51">
+        <v>36</v>
+      </c>
+      <c r="M51">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>33</v>
       </c>
       <c r="B52">
         <v>616</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52">
+        <v>541</v>
+      </c>
+      <c r="I52">
+        <v>37</v>
+      </c>
+      <c r="M52">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>34</v>
       </c>
       <c r="B53">
         <v>634</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53">
+        <v>543</v>
+      </c>
+      <c r="I53">
+        <v>38</v>
+      </c>
+      <c r="M53">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>35</v>
       </c>
       <c r="B54">
         <v>641</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54">
+        <v>547</v>
+      </c>
+      <c r="I54">
+        <v>39</v>
+      </c>
+      <c r="M54">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>36</v>
       </c>
       <c r="B55">
         <v>647</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>35</v>
+      </c>
+      <c r="F55">
+        <v>552</v>
+      </c>
+      <c r="I55">
+        <v>40</v>
+      </c>
+      <c r="M55">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>37</v>
       </c>
       <c r="B56">
         <v>665</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>36</v>
+      </c>
+      <c r="F56">
+        <v>568</v>
+      </c>
+      <c r="I56">
+        <v>41</v>
+      </c>
+      <c r="M56">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>38</v>
       </c>
       <c r="B57">
         <v>683</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>37</v>
+      </c>
+      <c r="F57">
+        <v>584</v>
+      </c>
+      <c r="I57">
+        <v>42</v>
+      </c>
+      <c r="M57">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>39</v>
       </c>
       <c r="B58">
         <v>689</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>38</v>
+      </c>
+      <c r="F58">
+        <v>594</v>
+      </c>
+      <c r="I58">
+        <v>43</v>
+      </c>
+      <c r="M58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>40</v>
       </c>
       <c r="B59">
         <v>701</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>39</v>
+      </c>
+      <c r="F59">
+        <v>612</v>
+      </c>
+      <c r="I59">
+        <v>44</v>
+      </c>
+      <c r="M59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>41</v>
       </c>
       <c r="B60">
         <v>718</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>40</v>
+      </c>
+      <c r="F60">
+        <v>623</v>
+      </c>
+      <c r="I60">
+        <v>45</v>
+      </c>
+      <c r="M60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>42</v>
       </c>
       <c r="B61">
         <v>725</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>41</v>
+      </c>
+      <c r="F61">
+        <v>631</v>
+      </c>
+      <c r="I61">
+        <v>46</v>
+      </c>
+      <c r="M61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>43</v>
       </c>
       <c r="B62">
         <v>742</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>42</v>
+      </c>
+      <c r="F62">
+        <v>640</v>
+      </c>
+      <c r="I62">
+        <v>47</v>
+      </c>
+      <c r="M62">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>44</v>
       </c>
       <c r="B63">
         <v>758</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>43</v>
+      </c>
+      <c r="F63">
+        <v>659</v>
+      </c>
+      <c r="I63">
+        <v>48</v>
+      </c>
+      <c r="M63">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>45</v>
       </c>
       <c r="B64">
         <v>773</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>44</v>
+      </c>
+      <c r="F64">
+        <v>677</v>
+      </c>
+      <c r="I64">
+        <v>49</v>
+      </c>
+      <c r="M64">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>46</v>
       </c>
       <c r="B65">
         <v>797</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>45</v>
+      </c>
+      <c r="F65">
+        <v>697</v>
+      </c>
+      <c r="I65">
+        <v>50</v>
+      </c>
+      <c r="M65">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>47</v>
       </c>
       <c r="B66">
         <v>819</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>46</v>
+      </c>
+      <c r="F66">
+        <v>719</v>
+      </c>
+      <c r="I66">
+        <v>51</v>
+      </c>
+      <c r="M66">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>48</v>
       </c>
       <c r="B67">
         <v>836</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>47</v>
+      </c>
+      <c r="F67">
+        <v>742</v>
+      </c>
+      <c r="I67">
+        <v>52</v>
+      </c>
+      <c r="M67">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>49</v>
       </c>
       <c r="B68">
         <v>848</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>48</v>
+      </c>
+      <c r="F68">
+        <v>754</v>
+      </c>
+      <c r="I68">
+        <v>53</v>
+      </c>
+      <c r="M68">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>50</v>
       </c>
       <c r="B69">
         <v>859</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>49</v>
+      </c>
+      <c r="F69">
+        <v>768</v>
+      </c>
+      <c r="I69">
+        <v>54</v>
+      </c>
+      <c r="M69">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>51</v>
       </c>
       <c r="B70">
         <v>864</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>50</v>
+      </c>
+      <c r="F70">
+        <v>790</v>
+      </c>
+      <c r="I70">
+        <v>55</v>
+      </c>
+      <c r="M70">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B71">
         <v>872</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>51</v>
+      </c>
+      <c r="F71">
+        <v>800</v>
+      </c>
+      <c r="I71">
+        <v>56</v>
+      </c>
+      <c r="M71">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B72">
         <v>877</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>52</v>
+      </c>
+      <c r="F72">
+        <v>810</v>
+      </c>
+      <c r="I72">
+        <v>57</v>
+      </c>
+      <c r="M72">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B73">
         <v>882</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>53</v>
+      </c>
+      <c r="F73">
+        <v>837</v>
+      </c>
+      <c r="I73" t="s">
+        <v>13</v>
+      </c>
+      <c r="M73">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>52</v>
       </c>
       <c r="B74">
         <v>892</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>54</v>
+      </c>
+      <c r="F74">
+        <v>847</v>
+      </c>
+      <c r="I74" t="s">
+        <v>14</v>
+      </c>
+      <c r="M74">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>53</v>
       </c>
       <c r="B75">
         <v>913</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>55</v>
+      </c>
+      <c r="F75">
+        <v>862</v>
+      </c>
+      <c r="I75" t="s">
+        <v>15</v>
+      </c>
+      <c r="M75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>54</v>
       </c>
       <c r="B76">
         <v>922</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>56</v>
+      </c>
+      <c r="F76">
+        <v>883</v>
+      </c>
+      <c r="I76">
+        <v>58</v>
+      </c>
+      <c r="M76">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>55</v>
       </c>
       <c r="B77">
         <v>940</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>57</v>
+      </c>
+      <c r="F77">
+        <v>900</v>
+      </c>
+      <c r="I77">
+        <v>59</v>
+      </c>
+      <c r="M77">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>56</v>
       </c>
       <c r="B78">
         <v>958</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>58</v>
+      </c>
+      <c r="F78">
+        <v>914</v>
+      </c>
+      <c r="I78">
+        <v>60</v>
+      </c>
+      <c r="M78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>57</v>
       </c>
       <c r="B79">
         <v>974</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79">
+        <v>923</v>
+      </c>
+      <c r="I79">
+        <v>61</v>
+      </c>
+      <c r="M79">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>58</v>
       </c>
       <c r="B80">
         <v>1001</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80">
+        <v>959</v>
+      </c>
+      <c r="I80">
+        <v>62</v>
+      </c>
+      <c r="M80">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>59</v>
       </c>
       <c r="B81">
         <v>1023</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81">
+        <v>962</v>
+      </c>
+      <c r="I81">
+        <v>63</v>
+      </c>
+      <c r="M81">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>60</v>
       </c>
       <c r="B82">
         <v>1043</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>59</v>
+      </c>
+      <c r="F82">
+        <v>979</v>
+      </c>
+      <c r="I82">
+        <v>64</v>
+      </c>
+      <c r="M82">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>61</v>
       </c>
       <c r="B83">
         <v>1057</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>60</v>
+      </c>
+      <c r="F83">
+        <v>990</v>
+      </c>
+      <c r="I83">
+        <v>65</v>
+      </c>
+      <c r="M83">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>62</v>
       </c>
       <c r="B84">
         <v>1068</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>61</v>
+      </c>
+      <c r="F84">
+        <v>1001</v>
+      </c>
+      <c r="I84">
+        <v>66</v>
+      </c>
+      <c r="M84">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>63</v>
       </c>
       <c r="B85">
         <v>1084</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>62</v>
+      </c>
+      <c r="F85">
+        <v>1008</v>
+      </c>
+      <c r="I85">
+        <v>67</v>
+      </c>
+      <c r="M85">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>64</v>
       </c>
       <c r="B86">
         <v>1091</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>63</v>
+      </c>
+      <c r="F86">
+        <v>1016</v>
+      </c>
+      <c r="I86">
+        <v>68</v>
+      </c>
+      <c r="M86">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>65</v>
       </c>
       <c r="B87">
         <v>1102</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>64</v>
+      </c>
+      <c r="F87">
+        <v>1035</v>
+      </c>
+      <c r="I87">
+        <v>69</v>
+      </c>
+      <c r="M87">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>66</v>
       </c>
       <c r="B88">
         <v>1114</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>65</v>
+      </c>
+      <c r="F88">
+        <v>1042</v>
+      </c>
+      <c r="I88">
+        <v>70</v>
+      </c>
+      <c r="M88">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>67</v>
       </c>
       <c r="B89">
         <v>1122</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>66</v>
+      </c>
+      <c r="F89">
+        <v>1049</v>
+      </c>
+      <c r="I89">
+        <v>71</v>
+      </c>
+      <c r="M89">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>68</v>
       </c>
       <c r="B90">
         <v>1145</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>67</v>
+      </c>
+      <c r="F90">
+        <v>1060</v>
+      </c>
+      <c r="I90">
+        <v>72</v>
+      </c>
+      <c r="M90">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>69</v>
       </c>
       <c r="B91">
         <v>1169</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>68</v>
+      </c>
+      <c r="F91">
+        <v>1081</v>
+      </c>
+      <c r="I91">
+        <v>73</v>
+      </c>
+      <c r="M91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>70</v>
       </c>
       <c r="B92">
         <v>1194</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>69</v>
+      </c>
+      <c r="F92">
+        <v>1105</v>
+      </c>
+      <c r="I92">
+        <v>74</v>
+      </c>
+      <c r="M92" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>71</v>
       </c>
       <c r="B93">
         <v>1202</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>70</v>
+      </c>
+      <c r="F93">
+        <v>1120</v>
+      </c>
+      <c r="I93">
+        <v>75</v>
+      </c>
+      <c r="M93" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>72</v>
       </c>
       <c r="B94">
         <v>1210</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>71</v>
+      </c>
+      <c r="F94">
+        <v>1137</v>
+      </c>
+      <c r="I94">
+        <v>76</v>
+      </c>
+      <c r="M94">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>73</v>
       </c>
       <c r="B95">
         <v>1214</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>72</v>
+      </c>
+      <c r="F95">
+        <v>1158</v>
+      </c>
+      <c r="I95">
+        <v>77</v>
+      </c>
+      <c r="M95">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>74</v>
       </c>
       <c r="B96">
         <v>1225</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>73</v>
+      </c>
+      <c r="F96">
+        <v>1172</v>
+      </c>
+      <c r="I96">
+        <v>78</v>
+      </c>
+      <c r="M96">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>75</v>
       </c>
       <c r="B97">
         <v>1229</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>74</v>
+      </c>
+      <c r="F97">
+        <v>1183</v>
+      </c>
+      <c r="I97">
+        <v>79</v>
+      </c>
+      <c r="M97">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>19</v>
       </c>
       <c r="B98">
         <v>1235</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>75</v>
+      </c>
+      <c r="F98">
+        <v>1193</v>
+      </c>
+      <c r="I98">
+        <v>80</v>
+      </c>
+      <c r="M98">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>20</v>
       </c>
       <c r="B99">
         <v>1239</v>
+      </c>
+      <c r="E99" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99">
+        <v>1209</v>
+      </c>
+      <c r="I99">
+        <v>81</v>
+      </c>
+      <c r="M99">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E100" t="s">
+        <v>25</v>
+      </c>
+      <c r="F100">
+        <v>1218</v>
+      </c>
+      <c r="I100">
+        <v>82</v>
+      </c>
+      <c r="M100">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>26</v>
+      </c>
+      <c r="F101">
+        <v>1221</v>
+      </c>
+      <c r="I101">
+        <v>83</v>
+      </c>
+      <c r="M101">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>76</v>
+      </c>
+      <c r="F102">
+        <v>1246</v>
+      </c>
+      <c r="I102">
+        <v>84</v>
+      </c>
+      <c r="M102">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>77</v>
+      </c>
+      <c r="F103">
+        <v>1265</v>
+      </c>
+      <c r="I103">
+        <v>85</v>
+      </c>
+      <c r="M103">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>78</v>
+      </c>
+      <c r="F104">
+        <v>1279</v>
+      </c>
+      <c r="I104">
+        <v>86</v>
+      </c>
+      <c r="M104">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>79</v>
+      </c>
+      <c r="F105">
+        <v>1291</v>
+      </c>
+      <c r="I105">
+        <v>87</v>
+      </c>
+      <c r="M105">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>80</v>
+      </c>
+      <c r="F106">
+        <v>1298</v>
+      </c>
+      <c r="I106" t="s">
+        <v>16</v>
+      </c>
+      <c r="M106">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>81</v>
+      </c>
+      <c r="F107">
+        <v>1310</v>
+      </c>
+      <c r="I107" t="s">
+        <v>17</v>
+      </c>
+      <c r="M107">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>82</v>
+      </c>
+      <c r="F108">
+        <v>1335</v>
+      </c>
+      <c r="I108" t="s">
+        <v>18</v>
+      </c>
+      <c r="M108">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>83</v>
+      </c>
+      <c r="F109">
+        <v>1351</v>
+      </c>
+      <c r="I109" t="s">
+        <v>22</v>
+      </c>
+      <c r="M109">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>84</v>
+      </c>
+      <c r="F110">
+        <v>1365</v>
+      </c>
+      <c r="I110" t="s">
+        <v>23</v>
+      </c>
+      <c r="M110">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>85</v>
+      </c>
+      <c r="F111">
+        <v>1377</v>
+      </c>
+      <c r="I111">
+        <v>88</v>
+      </c>
+      <c r="M111">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>86</v>
+      </c>
+      <c r="F112">
+        <v>1390</v>
+      </c>
+      <c r="I112">
+        <v>89</v>
+      </c>
+      <c r="M112">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="113" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>87</v>
+      </c>
+      <c r="F113">
+        <v>1412</v>
+      </c>
+      <c r="I113">
+        <v>90</v>
+      </c>
+      <c r="M113">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>88</v>
+      </c>
+      <c r="F114">
+        <v>1427</v>
+      </c>
+      <c r="I114">
+        <v>91</v>
+      </c>
+      <c r="M114">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="115" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>89</v>
+      </c>
+      <c r="F115">
+        <v>1442</v>
+      </c>
+      <c r="I115">
+        <v>92</v>
+      </c>
+      <c r="M115">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="116" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E116" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116">
+        <v>1456</v>
+      </c>
+      <c r="I116">
+        <v>93</v>
+      </c>
+      <c r="M116">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E117" t="s">
+        <v>20</v>
+      </c>
+      <c r="F117">
+        <v>1462</v>
+      </c>
+      <c r="I117">
+        <v>94</v>
+      </c>
+      <c r="M117">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I118">
+        <v>95</v>
+      </c>
+      <c r="M118">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="119" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I119">
+        <v>96</v>
+      </c>
+      <c r="M119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I120">
+        <v>97</v>
+      </c>
+      <c r="M120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I121">
+        <v>98</v>
+      </c>
+      <c r="M121" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I122">
+        <v>99</v>
+      </c>
+      <c r="M122">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="123" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I123">
+        <v>100</v>
+      </c>
+      <c r="M123">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="124" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I124">
+        <v>101</v>
+      </c>
+      <c r="M124">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="125" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I125">
+        <v>102</v>
+      </c>
+      <c r="M125">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="126" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I126">
+        <v>103</v>
+      </c>
+      <c r="M126">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I127">
+        <v>104</v>
+      </c>
+      <c r="M127">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="128" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="I128">
+        <v>105</v>
+      </c>
+      <c r="M128">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="129" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I129">
+        <v>106</v>
+      </c>
+      <c r="M129">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="130" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I130">
+        <v>107</v>
+      </c>
+      <c r="M130">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="131" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I131">
+        <v>108</v>
+      </c>
+      <c r="M131">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I132">
+        <v>109</v>
+      </c>
+      <c r="M132">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="133" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I133">
+        <v>110</v>
+      </c>
+      <c r="M133">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="134" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I134">
+        <v>111</v>
+      </c>
+      <c r="M134">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="135" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I135">
+        <v>112</v>
+      </c>
+      <c r="M135">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="136" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I136">
+        <v>113</v>
+      </c>
+      <c r="M136">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="137" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I137" t="s">
+        <v>24</v>
+      </c>
+      <c r="M137">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="138" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I138" t="s">
+        <v>25</v>
+      </c>
+      <c r="M138">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I139" t="s">
+        <v>26</v>
+      </c>
+      <c r="M139">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="140" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I140">
+        <v>114</v>
+      </c>
+      <c r="M140">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I141">
+        <v>115</v>
+      </c>
+      <c r="M141">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="142" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I142">
+        <v>116</v>
+      </c>
+      <c r="M142" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I143">
+        <v>117</v>
+      </c>
+      <c r="M143" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I144">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="145" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I145">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="146" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I146">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I147">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="148" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I148">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="149" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I149" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="150" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I150" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recorded pages numbers for book 3.
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE347A8-8E53-1F40-A6A3-1F282A2125D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C85DE3-0694-074C-BEE0-D9117C36B191}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t>Stormlight Achive Book Info</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Book 3 Chapter Pages (counting from 1)</t>
+  </si>
+  <si>
+    <t>(not the pdf pages)</t>
   </si>
 </sst>
 </file>
@@ -479,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G116" sqref="G116"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="J158" sqref="J158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,6 +569,11 @@
         <v>455891</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
@@ -623,6 +631,9 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
+      <c r="J12">
+        <v>14</v>
+      </c>
       <c r="M12" t="s">
         <v>9</v>
       </c>
@@ -643,6 +654,9 @@
       <c r="I13">
         <v>1</v>
       </c>
+      <c r="J13">
+        <v>27</v>
+      </c>
       <c r="M13">
         <v>1</v>
       </c>
@@ -663,6 +677,9 @@
       <c r="I14">
         <v>2</v>
       </c>
+      <c r="J14">
+        <v>35</v>
+      </c>
       <c r="M14">
         <v>2</v>
       </c>
@@ -683,6 +700,9 @@
       <c r="I15">
         <v>3</v>
       </c>
+      <c r="J15">
+        <v>47</v>
+      </c>
       <c r="M15">
         <v>3</v>
       </c>
@@ -703,6 +723,9 @@
       <c r="I16">
         <v>4</v>
       </c>
+      <c r="J16">
+        <v>61</v>
+      </c>
       <c r="M16">
         <v>4</v>
       </c>
@@ -723,6 +746,9 @@
       <c r="I17">
         <v>5</v>
       </c>
+      <c r="J17">
+        <v>79</v>
+      </c>
       <c r="M17">
         <v>5</v>
       </c>
@@ -743,6 +769,9 @@
       <c r="I18">
         <v>6</v>
       </c>
+      <c r="J18">
+        <v>87</v>
+      </c>
       <c r="M18">
         <v>6</v>
       </c>
@@ -763,6 +792,9 @@
       <c r="I19">
         <v>7</v>
       </c>
+      <c r="J19">
+        <v>96</v>
+      </c>
       <c r="M19">
         <v>7</v>
       </c>
@@ -783,6 +815,9 @@
       <c r="I20">
         <v>8</v>
       </c>
+      <c r="J20">
+        <v>113</v>
+      </c>
       <c r="M20">
         <v>8</v>
       </c>
@@ -803,6 +838,9 @@
       <c r="I21">
         <v>9</v>
       </c>
+      <c r="J21">
+        <v>125</v>
+      </c>
       <c r="M21">
         <v>9</v>
       </c>
@@ -823,6 +861,9 @@
       <c r="I22">
         <v>10</v>
       </c>
+      <c r="J22">
+        <v>131</v>
+      </c>
       <c r="M22">
         <v>10</v>
       </c>
@@ -843,6 +884,9 @@
       <c r="I23">
         <v>11</v>
       </c>
+      <c r="J23">
+        <v>147</v>
+      </c>
       <c r="M23">
         <v>11</v>
       </c>
@@ -863,6 +907,9 @@
       <c r="I24">
         <v>12</v>
       </c>
+      <c r="J24">
+        <v>166</v>
+      </c>
       <c r="M24">
         <v>12</v>
       </c>
@@ -883,6 +930,9 @@
       <c r="I25">
         <v>13</v>
       </c>
+      <c r="J25">
+        <v>187</v>
+      </c>
       <c r="M25">
         <v>13</v>
       </c>
@@ -903,6 +953,9 @@
       <c r="I26">
         <v>14</v>
       </c>
+      <c r="J26">
+        <v>200</v>
+      </c>
       <c r="M26">
         <v>14</v>
       </c>
@@ -923,6 +976,9 @@
       <c r="I27">
         <v>15</v>
       </c>
+      <c r="J27">
+        <v>205</v>
+      </c>
       <c r="M27">
         <v>15</v>
       </c>
@@ -943,6 +999,9 @@
       <c r="I28">
         <v>16</v>
       </c>
+      <c r="J28">
+        <v>217</v>
+      </c>
       <c r="M28">
         <v>16</v>
       </c>
@@ -963,6 +1022,9 @@
       <c r="I29">
         <v>17</v>
       </c>
+      <c r="J29">
+        <v>239</v>
+      </c>
       <c r="M29">
         <v>17</v>
       </c>
@@ -983,6 +1045,9 @@
       <c r="I30">
         <v>18</v>
       </c>
+      <c r="J30">
+        <v>250</v>
+      </c>
       <c r="M30">
         <v>18</v>
       </c>
@@ -1003,6 +1068,9 @@
       <c r="I31">
         <v>19</v>
       </c>
+      <c r="J31">
+        <v>273</v>
+      </c>
       <c r="M31">
         <v>19</v>
       </c>
@@ -1023,6 +1091,9 @@
       <c r="I32">
         <v>20</v>
       </c>
+      <c r="J32">
+        <v>287</v>
+      </c>
       <c r="M32" t="s">
         <v>10</v>
       </c>
@@ -1043,6 +1114,9 @@
       <c r="I33">
         <v>21</v>
       </c>
+      <c r="J33">
+        <v>292</v>
+      </c>
       <c r="M33" t="s">
         <v>11</v>
       </c>
@@ -1063,6 +1137,9 @@
       <c r="I34">
         <v>22</v>
       </c>
+      <c r="J34">
+        <v>305</v>
+      </c>
       <c r="M34" t="s">
         <v>12</v>
       </c>
@@ -1083,6 +1160,9 @@
       <c r="I35">
         <v>23</v>
       </c>
+      <c r="J35">
+        <v>313</v>
+      </c>
       <c r="M35">
         <v>20</v>
       </c>
@@ -1103,6 +1183,9 @@
       <c r="I36">
         <v>24</v>
       </c>
+      <c r="J36">
+        <v>319</v>
+      </c>
       <c r="M36">
         <v>21</v>
       </c>
@@ -1123,6 +1206,9 @@
       <c r="I37">
         <v>25</v>
       </c>
+      <c r="J37">
+        <v>334</v>
+      </c>
       <c r="M37">
         <v>22</v>
       </c>
@@ -1143,6 +1229,9 @@
       <c r="I38">
         <v>26</v>
       </c>
+      <c r="J38">
+        <v>347</v>
+      </c>
       <c r="M38">
         <v>23</v>
       </c>
@@ -1163,6 +1252,9 @@
       <c r="I39">
         <v>27</v>
       </c>
+      <c r="J39">
+        <v>365</v>
+      </c>
       <c r="M39">
         <v>24</v>
       </c>
@@ -1183,6 +1275,9 @@
       <c r="I40">
         <v>28</v>
       </c>
+      <c r="J40">
+        <v>378</v>
+      </c>
       <c r="M40">
         <v>25</v>
       </c>
@@ -1203,6 +1298,9 @@
       <c r="I41">
         <v>29</v>
       </c>
+      <c r="J41">
+        <v>393</v>
+      </c>
       <c r="M41">
         <v>26</v>
       </c>
@@ -1223,6 +1321,9 @@
       <c r="I42">
         <v>30</v>
       </c>
+      <c r="J42">
+        <v>415</v>
+      </c>
       <c r="M42">
         <v>27</v>
       </c>
@@ -1243,6 +1344,9 @@
       <c r="I43">
         <v>31</v>
       </c>
+      <c r="J43">
+        <v>419</v>
+      </c>
       <c r="M43">
         <v>28</v>
       </c>
@@ -1263,6 +1367,9 @@
       <c r="I44">
         <v>32</v>
       </c>
+      <c r="J44">
+        <v>436</v>
+      </c>
       <c r="M44">
         <v>29</v>
       </c>
@@ -1283,6 +1390,9 @@
       <c r="I45" t="s">
         <v>10</v>
       </c>
+      <c r="J45">
+        <v>442</v>
+      </c>
       <c r="M45">
         <v>30</v>
       </c>
@@ -1303,6 +1413,9 @@
       <c r="I46" t="s">
         <v>11</v>
       </c>
+      <c r="J46">
+        <v>445</v>
+      </c>
       <c r="M46">
         <v>31</v>
       </c>
@@ -1323,6 +1436,9 @@
       <c r="I47" t="s">
         <v>12</v>
       </c>
+      <c r="J47">
+        <v>452</v>
+      </c>
       <c r="M47">
         <v>32</v>
       </c>
@@ -1343,6 +1459,9 @@
       <c r="I48">
         <v>33</v>
       </c>
+      <c r="J48">
+        <v>461</v>
+      </c>
       <c r="M48">
         <v>33</v>
       </c>
@@ -1363,6 +1482,9 @@
       <c r="I49">
         <v>34</v>
       </c>
+      <c r="J49">
+        <v>468</v>
+      </c>
       <c r="M49">
         <v>34</v>
       </c>
@@ -1383,6 +1505,9 @@
       <c r="I50">
         <v>35</v>
       </c>
+      <c r="J50">
+        <v>484</v>
+      </c>
       <c r="M50">
         <v>35</v>
       </c>
@@ -1403,6 +1528,9 @@
       <c r="I51">
         <v>36</v>
       </c>
+      <c r="J51">
+        <v>498</v>
+      </c>
       <c r="M51">
         <v>36</v>
       </c>
@@ -1423,6 +1551,9 @@
       <c r="I52">
         <v>37</v>
       </c>
+      <c r="J52">
+        <v>505</v>
+      </c>
       <c r="M52">
         <v>37</v>
       </c>
@@ -1443,6 +1574,9 @@
       <c r="I53">
         <v>38</v>
       </c>
+      <c r="J53">
+        <v>530</v>
+      </c>
       <c r="M53">
         <v>38</v>
       </c>
@@ -1463,6 +1597,9 @@
       <c r="I54">
         <v>39</v>
       </c>
+      <c r="J54">
+        <v>550</v>
+      </c>
       <c r="M54">
         <v>39</v>
       </c>
@@ -1483,6 +1620,9 @@
       <c r="I55">
         <v>40</v>
       </c>
+      <c r="J55">
+        <v>563</v>
+      </c>
       <c r="M55">
         <v>40</v>
       </c>
@@ -1503,6 +1643,9 @@
       <c r="I56">
         <v>41</v>
       </c>
+      <c r="J56">
+        <v>575</v>
+      </c>
       <c r="M56">
         <v>41</v>
       </c>
@@ -1523,6 +1666,9 @@
       <c r="I57">
         <v>42</v>
       </c>
+      <c r="J57">
+        <v>582</v>
+      </c>
       <c r="M57">
         <v>42</v>
       </c>
@@ -1543,6 +1689,9 @@
       <c r="I58">
         <v>43</v>
       </c>
+      <c r="J58">
+        <v>590</v>
+      </c>
       <c r="M58">
         <v>43</v>
       </c>
@@ -1563,6 +1712,9 @@
       <c r="I59">
         <v>44</v>
       </c>
+      <c r="J59">
+        <v>599</v>
+      </c>
       <c r="M59" t="s">
         <v>13</v>
       </c>
@@ -1583,6 +1735,9 @@
       <c r="I60">
         <v>45</v>
       </c>
+      <c r="J60">
+        <v>614</v>
+      </c>
       <c r="M60" t="s">
         <v>14</v>
       </c>
@@ -1603,6 +1758,9 @@
       <c r="I61">
         <v>46</v>
       </c>
+      <c r="J61">
+        <v>623</v>
+      </c>
       <c r="M61" t="s">
         <v>15</v>
       </c>
@@ -1623,6 +1781,9 @@
       <c r="I62">
         <v>47</v>
       </c>
+      <c r="J62">
+        <v>638</v>
+      </c>
       <c r="M62">
         <v>44</v>
       </c>
@@ -1643,6 +1804,9 @@
       <c r="I63">
         <v>48</v>
       </c>
+      <c r="J63">
+        <v>645</v>
+      </c>
       <c r="M63">
         <v>45</v>
       </c>
@@ -1663,6 +1827,9 @@
       <c r="I64">
         <v>49</v>
       </c>
+      <c r="J64">
+        <v>652</v>
+      </c>
       <c r="M64">
         <v>46</v>
       </c>
@@ -1683,6 +1850,9 @@
       <c r="I65">
         <v>50</v>
       </c>
+      <c r="J65">
+        <v>667</v>
+      </c>
       <c r="M65">
         <v>47</v>
       </c>
@@ -1703,6 +1873,9 @@
       <c r="I66">
         <v>51</v>
       </c>
+      <c r="J66">
+        <v>680</v>
+      </c>
       <c r="M66">
         <v>48</v>
       </c>
@@ -1723,6 +1896,9 @@
       <c r="I67">
         <v>52</v>
       </c>
+      <c r="J67">
+        <v>689</v>
+      </c>
       <c r="M67">
         <v>49</v>
       </c>
@@ -1743,6 +1919,9 @@
       <c r="I68">
         <v>53</v>
       </c>
+      <c r="J68">
+        <v>699</v>
+      </c>
       <c r="M68">
         <v>50</v>
       </c>
@@ -1763,6 +1942,9 @@
       <c r="I69">
         <v>54</v>
       </c>
+      <c r="J69">
+        <v>712</v>
+      </c>
       <c r="M69">
         <v>51</v>
       </c>
@@ -1783,6 +1965,9 @@
       <c r="I70">
         <v>55</v>
       </c>
+      <c r="J70">
+        <v>722</v>
+      </c>
       <c r="M70">
         <v>52</v>
       </c>
@@ -1803,6 +1988,9 @@
       <c r="I71">
         <v>56</v>
       </c>
+      <c r="J71">
+        <v>732</v>
+      </c>
       <c r="M71">
         <v>53</v>
       </c>
@@ -1823,6 +2011,9 @@
       <c r="I72">
         <v>57</v>
       </c>
+      <c r="J72">
+        <v>740</v>
+      </c>
       <c r="M72">
         <v>54</v>
       </c>
@@ -1843,6 +2034,9 @@
       <c r="I73" t="s">
         <v>13</v>
       </c>
+      <c r="J73">
+        <v>749</v>
+      </c>
       <c r="M73">
         <v>55</v>
       </c>
@@ -1863,6 +2057,9 @@
       <c r="I74" t="s">
         <v>14</v>
       </c>
+      <c r="J74">
+        <v>760</v>
+      </c>
       <c r="M74">
         <v>56</v>
       </c>
@@ -1883,6 +2080,9 @@
       <c r="I75" t="s">
         <v>15</v>
       </c>
+      <c r="J75">
+        <v>771</v>
+      </c>
       <c r="M75">
         <v>57</v>
       </c>
@@ -1903,6 +2103,9 @@
       <c r="I76">
         <v>58</v>
       </c>
+      <c r="J76">
+        <v>781</v>
+      </c>
       <c r="M76">
         <v>58</v>
       </c>
@@ -1923,6 +2126,9 @@
       <c r="I77">
         <v>59</v>
       </c>
+      <c r="J77">
+        <v>789</v>
+      </c>
       <c r="M77">
         <v>59</v>
       </c>
@@ -1943,6 +2149,9 @@
       <c r="I78">
         <v>60</v>
       </c>
+      <c r="J78">
+        <v>807</v>
+      </c>
       <c r="M78">
         <v>60</v>
       </c>
@@ -1963,6 +2172,9 @@
       <c r="I79">
         <v>61</v>
       </c>
+      <c r="J79">
+        <v>817</v>
+      </c>
       <c r="M79">
         <v>61</v>
       </c>
@@ -1983,6 +2195,9 @@
       <c r="I80">
         <v>62</v>
       </c>
+      <c r="J80">
+        <v>833</v>
+      </c>
       <c r="M80">
         <v>62</v>
       </c>
@@ -2003,6 +2218,9 @@
       <c r="I81">
         <v>63</v>
       </c>
+      <c r="J81">
+        <v>847</v>
+      </c>
       <c r="M81">
         <v>63</v>
       </c>
@@ -2023,6 +2241,9 @@
       <c r="I82">
         <v>64</v>
       </c>
+      <c r="J82">
+        <v>858</v>
+      </c>
       <c r="M82">
         <v>64</v>
       </c>
@@ -2043,6 +2264,9 @@
       <c r="I83">
         <v>65</v>
       </c>
+      <c r="J83">
+        <v>869</v>
+      </c>
       <c r="M83">
         <v>65</v>
       </c>
@@ -2063,6 +2287,9 @@
       <c r="I84">
         <v>66</v>
       </c>
+      <c r="J84">
+        <v>886</v>
+      </c>
       <c r="M84">
         <v>66</v>
       </c>
@@ -2083,6 +2310,9 @@
       <c r="I85">
         <v>67</v>
       </c>
+      <c r="J85">
+        <v>897</v>
+      </c>
       <c r="M85">
         <v>67</v>
       </c>
@@ -2103,6 +2333,9 @@
       <c r="I86">
         <v>68</v>
       </c>
+      <c r="J86">
+        <v>912</v>
+      </c>
       <c r="M86">
         <v>68</v>
       </c>
@@ -2123,6 +2356,9 @@
       <c r="I87">
         <v>69</v>
       </c>
+      <c r="J87">
+        <v>924</v>
+      </c>
       <c r="M87">
         <v>69</v>
       </c>
@@ -2143,6 +2379,9 @@
       <c r="I88">
         <v>70</v>
       </c>
+      <c r="J88">
+        <v>934</v>
+      </c>
       <c r="M88">
         <v>70</v>
       </c>
@@ -2163,6 +2402,9 @@
       <c r="I89">
         <v>71</v>
       </c>
+      <c r="J89">
+        <v>943</v>
+      </c>
       <c r="M89">
         <v>71</v>
       </c>
@@ -2183,6 +2425,9 @@
       <c r="I90">
         <v>72</v>
       </c>
+      <c r="J90">
+        <v>955</v>
+      </c>
       <c r="M90">
         <v>72</v>
       </c>
@@ -2203,6 +2448,9 @@
       <c r="I91">
         <v>73</v>
       </c>
+      <c r="J91">
+        <v>969</v>
+      </c>
       <c r="M91" t="s">
         <v>16</v>
       </c>
@@ -2223,6 +2471,9 @@
       <c r="I92">
         <v>74</v>
       </c>
+      <c r="J92">
+        <v>982</v>
+      </c>
       <c r="M92" t="s">
         <v>17</v>
       </c>
@@ -2243,6 +2494,9 @@
       <c r="I93">
         <v>75</v>
       </c>
+      <c r="J93">
+        <v>992</v>
+      </c>
       <c r="M93" t="s">
         <v>18</v>
       </c>
@@ -2263,6 +2517,9 @@
       <c r="I94">
         <v>76</v>
       </c>
+      <c r="J94">
+        <v>1002</v>
+      </c>
       <c r="M94">
         <v>73</v>
       </c>
@@ -2283,6 +2540,9 @@
       <c r="I95">
         <v>77</v>
       </c>
+      <c r="J95">
+        <v>1015</v>
+      </c>
       <c r="M95">
         <v>74</v>
       </c>
@@ -2303,6 +2563,9 @@
       <c r="I96">
         <v>78</v>
       </c>
+      <c r="J96">
+        <v>1030</v>
+      </c>
       <c r="M96">
         <v>75</v>
       </c>
@@ -2323,6 +2586,9 @@
       <c r="I97">
         <v>79</v>
       </c>
+      <c r="J97">
+        <v>1043</v>
+      </c>
       <c r="M97">
         <v>76</v>
       </c>
@@ -2343,6 +2609,9 @@
       <c r="I98">
         <v>80</v>
       </c>
+      <c r="J98">
+        <v>1051</v>
+      </c>
       <c r="M98">
         <v>77</v>
       </c>
@@ -2363,6 +2632,9 @@
       <c r="I99">
         <v>81</v>
       </c>
+      <c r="J99">
+        <v>1057</v>
+      </c>
       <c r="M99">
         <v>78</v>
       </c>
@@ -2377,6 +2649,9 @@
       <c r="I100">
         <v>82</v>
       </c>
+      <c r="J100">
+        <v>1061</v>
+      </c>
       <c r="M100">
         <v>79</v>
       </c>
@@ -2391,6 +2666,9 @@
       <c r="I101">
         <v>83</v>
       </c>
+      <c r="J101">
+        <v>1073</v>
+      </c>
       <c r="M101">
         <v>80</v>
       </c>
@@ -2405,6 +2683,9 @@
       <c r="I102">
         <v>84</v>
       </c>
+      <c r="J102">
+        <v>1091</v>
+      </c>
       <c r="M102">
         <v>81</v>
       </c>
@@ -2419,6 +2700,9 @@
       <c r="I103">
         <v>85</v>
       </c>
+      <c r="J103">
+        <v>1106</v>
+      </c>
       <c r="M103">
         <v>82</v>
       </c>
@@ -2433,6 +2717,9 @@
       <c r="I104">
         <v>86</v>
       </c>
+      <c r="J104">
+        <v>1110</v>
+      </c>
       <c r="M104">
         <v>83</v>
       </c>
@@ -2447,6 +2734,9 @@
       <c r="I105">
         <v>87</v>
       </c>
+      <c r="J105">
+        <v>1116</v>
+      </c>
       <c r="M105">
         <v>84</v>
       </c>
@@ -2461,6 +2751,9 @@
       <c r="I106" t="s">
         <v>16</v>
       </c>
+      <c r="J106">
+        <v>1121</v>
+      </c>
       <c r="M106">
         <v>85</v>
       </c>
@@ -2475,6 +2768,9 @@
       <c r="I107" t="s">
         <v>17</v>
       </c>
+      <c r="J107">
+        <v>1129</v>
+      </c>
       <c r="M107">
         <v>86</v>
       </c>
@@ -2489,6 +2785,9 @@
       <c r="I108" t="s">
         <v>18</v>
       </c>
+      <c r="J108">
+        <v>1133</v>
+      </c>
       <c r="M108">
         <v>87</v>
       </c>
@@ -2503,6 +2802,9 @@
       <c r="I109" t="s">
         <v>22</v>
       </c>
+      <c r="J109">
+        <v>1135</v>
+      </c>
       <c r="M109">
         <v>88</v>
       </c>
@@ -2517,6 +2819,9 @@
       <c r="I110" t="s">
         <v>23</v>
       </c>
+      <c r="J110">
+        <v>1139</v>
+      </c>
       <c r="M110">
         <v>89</v>
       </c>
@@ -2531,6 +2836,9 @@
       <c r="I111">
         <v>88</v>
       </c>
+      <c r="J111">
+        <v>1145</v>
+      </c>
       <c r="M111">
         <v>90</v>
       </c>
@@ -2545,6 +2853,9 @@
       <c r="I112">
         <v>89</v>
       </c>
+      <c r="J112">
+        <v>1154</v>
+      </c>
       <c r="M112">
         <v>91</v>
       </c>
@@ -2559,6 +2870,9 @@
       <c r="I113">
         <v>90</v>
       </c>
+      <c r="J113">
+        <v>1167</v>
+      </c>
       <c r="M113">
         <v>92</v>
       </c>
@@ -2573,6 +2887,9 @@
       <c r="I114">
         <v>91</v>
       </c>
+      <c r="J114">
+        <v>1174</v>
+      </c>
       <c r="M114">
         <v>93</v>
       </c>
@@ -2587,6 +2904,9 @@
       <c r="I115">
         <v>92</v>
       </c>
+      <c r="J115">
+        <v>1181</v>
+      </c>
       <c r="M115">
         <v>94</v>
       </c>
@@ -2601,6 +2921,9 @@
       <c r="I116">
         <v>93</v>
       </c>
+      <c r="J116">
+        <v>1193</v>
+      </c>
       <c r="M116">
         <v>95</v>
       </c>
@@ -2615,6 +2938,9 @@
       <c r="I117">
         <v>94</v>
       </c>
+      <c r="J117">
+        <v>1201</v>
+      </c>
       <c r="M117">
         <v>96</v>
       </c>
@@ -2623,6 +2949,9 @@
       <c r="I118">
         <v>95</v>
       </c>
+      <c r="J118">
+        <v>1205</v>
+      </c>
       <c r="M118">
         <v>97</v>
       </c>
@@ -2631,6 +2960,9 @@
       <c r="I119">
         <v>96</v>
       </c>
+      <c r="J119">
+        <v>1211</v>
+      </c>
       <c r="M119" t="s">
         <v>22</v>
       </c>
@@ -2639,6 +2971,9 @@
       <c r="I120">
         <v>97</v>
       </c>
+      <c r="J120">
+        <v>1226</v>
+      </c>
       <c r="M120" t="s">
         <v>23</v>
       </c>
@@ -2647,6 +2982,9 @@
       <c r="I121">
         <v>98</v>
       </c>
+      <c r="J121">
+        <v>1241</v>
+      </c>
       <c r="M121" t="s">
         <v>24</v>
       </c>
@@ -2655,6 +2993,9 @@
       <c r="I122">
         <v>99</v>
       </c>
+      <c r="J122">
+        <v>1251</v>
+      </c>
       <c r="M122">
         <v>98</v>
       </c>
@@ -2663,6 +3004,9 @@
       <c r="I123">
         <v>100</v>
       </c>
+      <c r="J123">
+        <v>1264</v>
+      </c>
       <c r="M123">
         <v>99</v>
       </c>
@@ -2671,6 +3015,9 @@
       <c r="I124">
         <v>101</v>
       </c>
+      <c r="J124">
+        <v>1277</v>
+      </c>
       <c r="M124">
         <v>100</v>
       </c>
@@ -2679,6 +3026,9 @@
       <c r="I125">
         <v>102</v>
       </c>
+      <c r="J125">
+        <v>1286</v>
+      </c>
       <c r="M125">
         <v>101</v>
       </c>
@@ -2687,6 +3037,9 @@
       <c r="I126">
         <v>103</v>
       </c>
+      <c r="J126">
+        <v>1302</v>
+      </c>
       <c r="M126">
         <v>102</v>
       </c>
@@ -2695,6 +3048,9 @@
       <c r="I127">
         <v>104</v>
       </c>
+      <c r="J127">
+        <v>1313</v>
+      </c>
       <c r="M127">
         <v>103</v>
       </c>
@@ -2703,6 +3059,9 @@
       <c r="I128">
         <v>105</v>
       </c>
+      <c r="J128">
+        <v>1323</v>
+      </c>
       <c r="M128">
         <v>104</v>
       </c>
@@ -2711,6 +3070,9 @@
       <c r="I129">
         <v>106</v>
       </c>
+      <c r="J129">
+        <v>1333</v>
+      </c>
       <c r="M129">
         <v>105</v>
       </c>
@@ -2719,6 +3081,9 @@
       <c r="I130">
         <v>107</v>
       </c>
+      <c r="J130">
+        <v>1340</v>
+      </c>
       <c r="M130">
         <v>106</v>
       </c>
@@ -2727,6 +3092,9 @@
       <c r="I131">
         <v>108</v>
       </c>
+      <c r="J131">
+        <v>1362</v>
+      </c>
       <c r="M131">
         <v>107</v>
       </c>
@@ -2735,6 +3103,9 @@
       <c r="I132">
         <v>109</v>
       </c>
+      <c r="J132">
+        <v>1382</v>
+      </c>
       <c r="M132">
         <v>108</v>
       </c>
@@ -2743,6 +3114,9 @@
       <c r="I133">
         <v>110</v>
       </c>
+      <c r="J133">
+        <v>1396</v>
+      </c>
       <c r="M133">
         <v>109</v>
       </c>
@@ -2751,6 +3125,9 @@
       <c r="I134">
         <v>111</v>
       </c>
+      <c r="J134">
+        <v>1403</v>
+      </c>
       <c r="M134">
         <v>110</v>
       </c>
@@ -2759,6 +3136,9 @@
       <c r="I135">
         <v>112</v>
       </c>
+      <c r="J135">
+        <v>1418</v>
+      </c>
       <c r="M135">
         <v>111</v>
       </c>
@@ -2767,6 +3147,9 @@
       <c r="I136">
         <v>113</v>
       </c>
+      <c r="J136">
+        <v>1423</v>
+      </c>
       <c r="M136">
         <v>112</v>
       </c>
@@ -2775,6 +3158,9 @@
       <c r="I137" t="s">
         <v>24</v>
       </c>
+      <c r="J137">
+        <v>1431</v>
+      </c>
       <c r="M137">
         <v>113</v>
       </c>
@@ -2783,6 +3169,9 @@
       <c r="I138" t="s">
         <v>25</v>
       </c>
+      <c r="J138">
+        <v>1434</v>
+      </c>
       <c r="M138">
         <v>114</v>
       </c>
@@ -2791,6 +3180,9 @@
       <c r="I139" t="s">
         <v>26</v>
       </c>
+      <c r="J139">
+        <v>1448</v>
+      </c>
       <c r="M139">
         <v>115</v>
       </c>
@@ -2799,6 +3191,9 @@
       <c r="I140">
         <v>114</v>
       </c>
+      <c r="J140">
+        <v>1452</v>
+      </c>
       <c r="M140">
         <v>116</v>
       </c>
@@ -2807,6 +3202,9 @@
       <c r="I141">
         <v>115</v>
       </c>
+      <c r="J141">
+        <v>1464</v>
+      </c>
       <c r="M141">
         <v>117</v>
       </c>
@@ -2815,6 +3213,9 @@
       <c r="I142">
         <v>116</v>
       </c>
+      <c r="J142">
+        <v>1480</v>
+      </c>
       <c r="M142" t="s">
         <v>19</v>
       </c>
@@ -2823,6 +3224,9 @@
       <c r="I143">
         <v>117</v>
       </c>
+      <c r="J143">
+        <v>1499</v>
+      </c>
       <c r="M143" t="s">
         <v>20</v>
       </c>
@@ -2831,35 +3235,56 @@
       <c r="I144">
         <v>118</v>
       </c>
-    </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J144">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I145">
         <v>119</v>
       </c>
-    </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J145">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I146">
         <v>120</v>
       </c>
-    </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J146">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I147">
         <v>121</v>
       </c>
-    </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J147">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I148">
         <v>122</v>
       </c>
-    </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J148">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I149" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="J149">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I150" t="s">
         <v>20</v>
+      </c>
+      <c r="J150">
+        <v>1668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recorded pages numbers for book 4.
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C85DE3-0694-074C-BEE0-D9117C36B191}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC073A-2311-DB49-BBFE-59FC09B60F24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
   <si>
     <t>Stormlight Achive Book Info</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>(not the pdf pages)</t>
+  </si>
+  <si>
+    <t>Book 4 Chapter Pages (counting from 1)</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="J158" sqref="J158"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="N145" sqref="N145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +589,7 @@
         <v>27</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -637,6 +640,9 @@
       <c r="M12" t="s">
         <v>9</v>
       </c>
+      <c r="N12">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -660,6 +666,9 @@
       <c r="M13">
         <v>1</v>
       </c>
+      <c r="N13">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -683,6 +692,9 @@
       <c r="M14">
         <v>2</v>
       </c>
+      <c r="N14">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -706,6 +718,9 @@
       <c r="M15">
         <v>3</v>
       </c>
+      <c r="N15">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -729,8 +744,11 @@
       <c r="M16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -752,8 +770,11 @@
       <c r="M17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -775,8 +796,11 @@
       <c r="M18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -798,8 +822,11 @@
       <c r="M19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -821,8 +848,11 @@
       <c r="M20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -844,8 +874,11 @@
       <c r="M21">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -867,8 +900,11 @@
       <c r="M22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -890,8 +926,11 @@
       <c r="M23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
@@ -913,8 +952,11 @@
       <c r="M24">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -936,8 +978,11 @@
       <c r="M25">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -959,8 +1004,11 @@
       <c r="M26">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -982,8 +1030,11 @@
       <c r="M27">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
@@ -1005,8 +1056,11 @@
       <c r="M28">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>13</v>
       </c>
@@ -1028,8 +1082,11 @@
       <c r="M29">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>14</v>
       </c>
@@ -1051,8 +1108,11 @@
       <c r="M30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -1074,8 +1134,11 @@
       <c r="M31">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>
@@ -1097,8 +1160,11 @@
       <c r="M32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>17</v>
       </c>
@@ -1120,8 +1186,11 @@
       <c r="M33" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>18</v>
       </c>
@@ -1143,8 +1212,11 @@
       <c r="M34" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>19</v>
       </c>
@@ -1166,8 +1238,11 @@
       <c r="M35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
@@ -1189,8 +1264,11 @@
       <c r="M36">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>21</v>
       </c>
@@ -1212,8 +1290,11 @@
       <c r="M37">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>22</v>
       </c>
@@ -1235,8 +1316,11 @@
       <c r="M38">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>23</v>
       </c>
@@ -1258,8 +1342,11 @@
       <c r="M39">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>24</v>
       </c>
@@ -1281,8 +1368,11 @@
       <c r="M40">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>25</v>
       </c>
@@ -1304,8 +1394,11 @@
       <c r="M41">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>26</v>
       </c>
@@ -1327,8 +1420,11 @@
       <c r="M42">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>27</v>
       </c>
@@ -1350,8 +1446,11 @@
       <c r="M43">
         <v>28</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>28</v>
       </c>
@@ -1373,8 +1472,11 @@
       <c r="M44">
         <v>29</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1396,8 +1498,11 @@
       <c r="M45">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1419,8 +1524,11 @@
       <c r="M46">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1442,8 +1550,11 @@
       <c r="M47">
         <v>32</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>29</v>
       </c>
@@ -1465,8 +1576,11 @@
       <c r="M48">
         <v>33</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>30</v>
       </c>
@@ -1488,8 +1602,11 @@
       <c r="M49">
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>31</v>
       </c>
@@ -1511,8 +1628,11 @@
       <c r="M50">
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N50">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>32</v>
       </c>
@@ -1534,8 +1654,11 @@
       <c r="M51">
         <v>36</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>33</v>
       </c>
@@ -1557,8 +1680,11 @@
       <c r="M52">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>34</v>
       </c>
@@ -1580,8 +1706,11 @@
       <c r="M53">
         <v>38</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>35</v>
       </c>
@@ -1603,8 +1732,11 @@
       <c r="M54">
         <v>39</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>36</v>
       </c>
@@ -1626,8 +1758,11 @@
       <c r="M55">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N55">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>37</v>
       </c>
@@ -1649,8 +1784,11 @@
       <c r="M56">
         <v>41</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N56">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>38</v>
       </c>
@@ -1672,8 +1810,11 @@
       <c r="M57">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N57">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>39</v>
       </c>
@@ -1695,8 +1836,11 @@
       <c r="M58">
         <v>43</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N58">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>40</v>
       </c>
@@ -1718,8 +1862,11 @@
       <c r="M59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N59">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>41</v>
       </c>
@@ -1741,8 +1888,11 @@
       <c r="M60" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N60">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>42</v>
       </c>
@@ -1764,8 +1914,11 @@
       <c r="M61" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>43</v>
       </c>
@@ -1787,8 +1940,11 @@
       <c r="M62">
         <v>44</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>44</v>
       </c>
@@ -1810,8 +1966,11 @@
       <c r="M63">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>45</v>
       </c>
@@ -1833,8 +1992,11 @@
       <c r="M64">
         <v>46</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N64">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>46</v>
       </c>
@@ -1856,8 +2018,11 @@
       <c r="M65">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>47</v>
       </c>
@@ -1879,8 +2044,11 @@
       <c r="M66">
         <v>48</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N66">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>48</v>
       </c>
@@ -1902,8 +2070,11 @@
       <c r="M67">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N67">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>49</v>
       </c>
@@ -1925,8 +2096,11 @@
       <c r="M68">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>50</v>
       </c>
@@ -1948,8 +2122,11 @@
       <c r="M69">
         <v>51</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N69">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>51</v>
       </c>
@@ -1971,8 +2148,11 @@
       <c r="M70">
         <v>52</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N70">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>16</v>
       </c>
@@ -1994,8 +2174,11 @@
       <c r="M71">
         <v>53</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N71">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -2017,8 +2200,11 @@
       <c r="M72">
         <v>54</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N72">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -2040,8 +2226,11 @@
       <c r="M73">
         <v>55</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N73">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>52</v>
       </c>
@@ -2063,8 +2252,11 @@
       <c r="M74">
         <v>56</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N74">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>53</v>
       </c>
@@ -2086,8 +2278,11 @@
       <c r="M75">
         <v>57</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>54</v>
       </c>
@@ -2109,8 +2304,11 @@
       <c r="M76">
         <v>58</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N76">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>55</v>
       </c>
@@ -2132,8 +2330,11 @@
       <c r="M77">
         <v>59</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N77">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>56</v>
       </c>
@@ -2155,8 +2356,11 @@
       <c r="M78">
         <v>60</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N78">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>57</v>
       </c>
@@ -2178,8 +2382,11 @@
       <c r="M79">
         <v>61</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N79">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>58</v>
       </c>
@@ -2201,8 +2408,11 @@
       <c r="M80">
         <v>62</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N80">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>59</v>
       </c>
@@ -2224,8 +2434,11 @@
       <c r="M81">
         <v>63</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N81">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>60</v>
       </c>
@@ -2247,8 +2460,11 @@
       <c r="M82">
         <v>64</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>61</v>
       </c>
@@ -2270,8 +2486,11 @@
       <c r="M83">
         <v>65</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N83">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>62</v>
       </c>
@@ -2293,8 +2512,11 @@
       <c r="M84">
         <v>66</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>63</v>
       </c>
@@ -2316,8 +2538,11 @@
       <c r="M85">
         <v>67</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N85">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>64</v>
       </c>
@@ -2339,8 +2564,11 @@
       <c r="M86">
         <v>68</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N86">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>65</v>
       </c>
@@ -2362,8 +2590,11 @@
       <c r="M87">
         <v>69</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N87">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>66</v>
       </c>
@@ -2385,8 +2616,11 @@
       <c r="M88">
         <v>70</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N88">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>67</v>
       </c>
@@ -2408,8 +2642,11 @@
       <c r="M89">
         <v>71</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N89">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>68</v>
       </c>
@@ -2431,8 +2668,11 @@
       <c r="M90">
         <v>72</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N90">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>69</v>
       </c>
@@ -2454,8 +2694,11 @@
       <c r="M91" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N91">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>70</v>
       </c>
@@ -2477,8 +2720,11 @@
       <c r="M92" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>71</v>
       </c>
@@ -2500,8 +2746,11 @@
       <c r="M93" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N93">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>72</v>
       </c>
@@ -2523,8 +2772,11 @@
       <c r="M94">
         <v>73</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N94">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>73</v>
       </c>
@@ -2546,8 +2798,11 @@
       <c r="M95">
         <v>74</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N95">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>74</v>
       </c>
@@ -2569,8 +2824,11 @@
       <c r="M96">
         <v>75</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N96">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>75</v>
       </c>
@@ -2592,8 +2850,11 @@
       <c r="M97">
         <v>76</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N97">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>19</v>
       </c>
@@ -2615,8 +2876,11 @@
       <c r="M98">
         <v>77</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -2638,8 +2902,11 @@
       <c r="M99">
         <v>78</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N99">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
         <v>25</v>
       </c>
@@ -2655,8 +2922,11 @@
       <c r="M100">
         <v>79</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N100">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E101" t="s">
         <v>26</v>
       </c>
@@ -2672,8 +2942,11 @@
       <c r="M101">
         <v>80</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N101">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E102">
         <v>76</v>
       </c>
@@ -2689,8 +2962,11 @@
       <c r="M102">
         <v>81</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N102">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E103">
         <v>77</v>
       </c>
@@ -2706,8 +2982,11 @@
       <c r="M103">
         <v>82</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N103">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E104">
         <v>78</v>
       </c>
@@ -2723,8 +3002,11 @@
       <c r="M104">
         <v>83</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N104">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E105">
         <v>79</v>
       </c>
@@ -2740,8 +3022,11 @@
       <c r="M105">
         <v>84</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N105">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E106">
         <v>80</v>
       </c>
@@ -2757,8 +3042,11 @@
       <c r="M106">
         <v>85</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N106">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E107">
         <v>81</v>
       </c>
@@ -2774,8 +3062,11 @@
       <c r="M107">
         <v>86</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N107">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E108">
         <v>82</v>
       </c>
@@ -2791,8 +3082,11 @@
       <c r="M108">
         <v>87</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N108">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E109">
         <v>83</v>
       </c>
@@ -2808,8 +3102,11 @@
       <c r="M109">
         <v>88</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N109">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E110">
         <v>84</v>
       </c>
@@ -2825,8 +3122,11 @@
       <c r="M110">
         <v>89</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N110">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E111">
         <v>85</v>
       </c>
@@ -2842,8 +3142,11 @@
       <c r="M111">
         <v>90</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N111">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E112">
         <v>86</v>
       </c>
@@ -2859,8 +3162,11 @@
       <c r="M112">
         <v>91</v>
       </c>
-    </row>
-    <row r="113" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N112">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="113" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E113">
         <v>87</v>
       </c>
@@ -2876,8 +3182,11 @@
       <c r="M113">
         <v>92</v>
       </c>
-    </row>
-    <row r="114" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N113">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="114" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E114">
         <v>88</v>
       </c>
@@ -2893,8 +3202,11 @@
       <c r="M114">
         <v>93</v>
       </c>
-    </row>
-    <row r="115" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N114">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="115" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E115">
         <v>89</v>
       </c>
@@ -2910,8 +3222,11 @@
       <c r="M115">
         <v>94</v>
       </c>
-    </row>
-    <row r="116" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N115">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="116" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E116" t="s">
         <v>19</v>
       </c>
@@ -2927,8 +3242,11 @@
       <c r="M116">
         <v>95</v>
       </c>
-    </row>
-    <row r="117" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N116">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="117" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E117" t="s">
         <v>20</v>
       </c>
@@ -2944,8 +3262,11 @@
       <c r="M117">
         <v>96</v>
       </c>
-    </row>
-    <row r="118" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N117">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="118" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I118">
         <v>95</v>
       </c>
@@ -2955,8 +3276,11 @@
       <c r="M118">
         <v>97</v>
       </c>
-    </row>
-    <row r="119" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N118">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="119" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I119">
         <v>96</v>
       </c>
@@ -2966,8 +3290,11 @@
       <c r="M119" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="120" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N119">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="120" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I120">
         <v>97</v>
       </c>
@@ -2977,8 +3304,11 @@
       <c r="M120" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="121" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N120">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="121" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I121">
         <v>98</v>
       </c>
@@ -2988,8 +3318,11 @@
       <c r="M121" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="122" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N121">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="122" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I122">
         <v>99</v>
       </c>
@@ -2999,8 +3332,11 @@
       <c r="M122">
         <v>98</v>
       </c>
-    </row>
-    <row r="123" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N122">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="123" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I123">
         <v>100</v>
       </c>
@@ -3010,8 +3346,11 @@
       <c r="M123">
         <v>99</v>
       </c>
-    </row>
-    <row r="124" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N123">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="124" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I124">
         <v>101</v>
       </c>
@@ -3021,8 +3360,11 @@
       <c r="M124">
         <v>100</v>
       </c>
-    </row>
-    <row r="125" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N124">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="125" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I125">
         <v>102</v>
       </c>
@@ -3032,8 +3374,11 @@
       <c r="M125">
         <v>101</v>
       </c>
-    </row>
-    <row r="126" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N125">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="126" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I126">
         <v>103</v>
       </c>
@@ -3043,8 +3388,11 @@
       <c r="M126">
         <v>102</v>
       </c>
-    </row>
-    <row r="127" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N126">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="127" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I127">
         <v>104</v>
       </c>
@@ -3054,8 +3402,11 @@
       <c r="M127">
         <v>103</v>
       </c>
-    </row>
-    <row r="128" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="N127">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="128" spans="5:14" x14ac:dyDescent="0.2">
       <c r="I128">
         <v>105</v>
       </c>
@@ -3065,8 +3416,11 @@
       <c r="M128">
         <v>104</v>
       </c>
-    </row>
-    <row r="129" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N128">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="129" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I129">
         <v>106</v>
       </c>
@@ -3076,8 +3430,11 @@
       <c r="M129">
         <v>105</v>
       </c>
-    </row>
-    <row r="130" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N129">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="130" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I130">
         <v>107</v>
       </c>
@@ -3087,8 +3444,11 @@
       <c r="M130">
         <v>106</v>
       </c>
-    </row>
-    <row r="131" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N130">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="131" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I131">
         <v>108</v>
       </c>
@@ -3098,8 +3458,11 @@
       <c r="M131">
         <v>107</v>
       </c>
-    </row>
-    <row r="132" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N131">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="132" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I132">
         <v>109</v>
       </c>
@@ -3109,8 +3472,11 @@
       <c r="M132">
         <v>108</v>
       </c>
-    </row>
-    <row r="133" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N132">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="133" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I133">
         <v>110</v>
       </c>
@@ -3120,8 +3486,11 @@
       <c r="M133">
         <v>109</v>
       </c>
-    </row>
-    <row r="134" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N133">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="134" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I134">
         <v>111</v>
       </c>
@@ -3131,8 +3500,11 @@
       <c r="M134">
         <v>110</v>
       </c>
-    </row>
-    <row r="135" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N134">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="135" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I135">
         <v>112</v>
       </c>
@@ -3142,8 +3514,11 @@
       <c r="M135">
         <v>111</v>
       </c>
-    </row>
-    <row r="136" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N135">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="136" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I136">
         <v>113</v>
       </c>
@@ -3153,8 +3528,11 @@
       <c r="M136">
         <v>112</v>
       </c>
-    </row>
-    <row r="137" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N136">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="137" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I137" t="s">
         <v>24</v>
       </c>
@@ -3164,8 +3542,11 @@
       <c r="M137">
         <v>113</v>
       </c>
-    </row>
-    <row r="138" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N137">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="138" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I138" t="s">
         <v>25</v>
       </c>
@@ -3175,8 +3556,11 @@
       <c r="M138">
         <v>114</v>
       </c>
-    </row>
-    <row r="139" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N138">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="139" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I139" t="s">
         <v>26</v>
       </c>
@@ -3186,8 +3570,11 @@
       <c r="M139">
         <v>115</v>
       </c>
-    </row>
-    <row r="140" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N139">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="140" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I140">
         <v>114</v>
       </c>
@@ -3197,8 +3584,11 @@
       <c r="M140">
         <v>116</v>
       </c>
-    </row>
-    <row r="141" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N140">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="141" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I141">
         <v>115</v>
       </c>
@@ -3208,8 +3598,11 @@
       <c r="M141">
         <v>117</v>
       </c>
-    </row>
-    <row r="142" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N141">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="142" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I142">
         <v>116</v>
       </c>
@@ -3219,8 +3612,11 @@
       <c r="M142" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="143" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N142">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="143" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I143">
         <v>117</v>
       </c>
@@ -3230,8 +3626,11 @@
       <c r="M143" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="144" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="N143">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="144" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I144">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Recorded book unit numbers (chapters + prologues and intervals, etc.)
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC073A-2311-DB49-BBFE-59FC09B60F24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859520E4-4881-6342-AA48-0060C1A837F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
+    <workbookView xWindow="1260" yWindow="-18180" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
   <si>
     <t>Stormlight Achive Book Info</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Book 4 Chapter Pages (counting from 1)</t>
+  </si>
+  <si>
+    <t>Book Units</t>
   </si>
 </sst>
 </file>
@@ -485,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="N145" sqref="N145"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,6 +518,9 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -529,6 +535,9 @@
       <c r="D4">
         <v>383389</v>
       </c>
+      <c r="E4">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -543,6 +552,9 @@
       <c r="D5">
         <v>399431</v>
       </c>
+      <c r="E5">
+        <v>105</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -557,6 +569,9 @@
       <c r="D6">
         <v>451912</v>
       </c>
+      <c r="E6">
+        <v>136</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -570,6 +585,9 @@
       </c>
       <c r="D7">
         <v>455891</v>
+      </c>
+      <c r="E7">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Processed all books, saved file into pickled dataframe sla_chapter_text.pkl.
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859520E4-4881-6342-AA48-0060C1A837F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68898AA-BAFA-5045-8B7F-3A75C7CA5087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-18180" windowWidth="25440" windowHeight="15000" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
   <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Started some more work on sentiment analysis in the main notebook.
</commit_message>
<xml_diff>
--- a/StormlightArchiveBooks/BookPageInfo.xlsx
+++ b/StormlightArchiveBooks/BookPageInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/DataScience/Metis/MetisProjects/StormlightArchiveNLP/StormlightArchiveBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68898AA-BAFA-5045-8B7F-3A75C7CA5087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E842055C-C066-EA4C-9B62-93A682510A88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{B48DE19F-367A-F04E-A19E-E166575449E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <t>Stormlight Achive Book Info</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Book Units</t>
+  </si>
+  <si>
+    <t>Global Chapter Number</t>
   </si>
 </sst>
 </file>
@@ -486,26 +489,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE19ADBE-0769-7D44-8078-61239A38457F}">
-  <dimension ref="A1:N150"/>
+  <dimension ref="A1:O150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="G119" workbookViewId="0">
+      <selection activeCell="Q132" sqref="Q132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
     <col min="14" max="14" width="12.5" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -522,7 +529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -539,7 +546,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -556,7 +563,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -573,7 +580,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -590,12 +597,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -610,2295 +617,3351 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="M11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12">
         <v>21</v>
       </c>
+      <c r="G12">
+        <v>88</v>
+      </c>
       <c r="I12" t="s">
         <v>9</v>
       </c>
       <c r="J12">
         <v>14</v>
       </c>
+      <c r="K12">
+        <v>193</v>
+      </c>
       <c r="M12" t="s">
         <v>9</v>
       </c>
       <c r="N12">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <v>18</v>
       </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
         <v>41</v>
       </c>
+      <c r="G13">
+        <v>89</v>
+      </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13">
         <v>27</v>
       </c>
+      <c r="K13">
+        <v>194</v>
+      </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
         <v>37</v>
       </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <v>67</v>
       </c>
+      <c r="G14">
+        <v>90</v>
+      </c>
       <c r="I14">
         <v>2</v>
       </c>
       <c r="J14">
         <v>35</v>
       </c>
+      <c r="K14">
+        <v>195</v>
+      </c>
       <c r="M14">
         <v>2</v>
       </c>
       <c r="N14">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
         <v>51</v>
       </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15">
         <v>86</v>
       </c>
+      <c r="G15">
+        <v>91</v>
+      </c>
       <c r="I15">
         <v>3</v>
       </c>
       <c r="J15">
         <v>47</v>
       </c>
+      <c r="K15">
+        <v>196</v>
+      </c>
       <c r="M15">
         <v>3</v>
       </c>
       <c r="N15">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16">
         <v>67</v>
       </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
       <c r="E16">
         <v>4</v>
       </c>
       <c r="F16">
         <v>96</v>
       </c>
+      <c r="G16">
+        <v>92</v>
+      </c>
       <c r="I16">
         <v>4</v>
       </c>
       <c r="J16">
         <v>61</v>
       </c>
+      <c r="K16">
+        <v>197</v>
+      </c>
       <c r="M16">
         <v>4</v>
       </c>
       <c r="N16">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17">
         <v>83</v>
       </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
         <v>112</v>
       </c>
+      <c r="G17">
+        <v>93</v>
+      </c>
       <c r="I17">
         <v>5</v>
       </c>
       <c r="J17">
         <v>79</v>
       </c>
+      <c r="K17">
+        <v>198</v>
+      </c>
       <c r="M17">
         <v>5</v>
       </c>
       <c r="N17">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
         <v>96</v>
       </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
       <c r="E18">
         <v>6</v>
       </c>
       <c r="F18">
         <v>140</v>
       </c>
+      <c r="G18">
+        <v>94</v>
+      </c>
       <c r="I18">
         <v>6</v>
       </c>
       <c r="J18">
         <v>87</v>
       </c>
+      <c r="K18">
+        <v>199</v>
+      </c>
       <c r="M18">
         <v>6</v>
       </c>
       <c r="N18">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19">
         <v>110</v>
       </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
       <c r="E19">
         <v>7</v>
       </c>
       <c r="F19">
         <v>155</v>
       </c>
+      <c r="G19">
+        <v>95</v>
+      </c>
       <c r="I19">
         <v>7</v>
       </c>
       <c r="J19">
         <v>96</v>
       </c>
+      <c r="K19">
+        <v>200</v>
+      </c>
       <c r="M19">
         <v>7</v>
       </c>
       <c r="N19">
         <v>131</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
         <v>132</v>
       </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
       <c r="E20">
         <v>8</v>
       </c>
       <c r="F20">
         <v>164</v>
       </c>
+      <c r="G20">
+        <v>96</v>
+      </c>
       <c r="I20">
         <v>8</v>
       </c>
       <c r="J20">
         <v>113</v>
       </c>
+      <c r="K20">
+        <v>201</v>
+      </c>
       <c r="M20">
         <v>8</v>
       </c>
       <c r="N20">
         <v>148</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
       <c r="B21">
         <v>151</v>
       </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
       <c r="E21">
         <v>9</v>
       </c>
       <c r="F21">
         <v>174</v>
       </c>
+      <c r="G21">
+        <v>97</v>
+      </c>
       <c r="I21">
         <v>9</v>
       </c>
       <c r="J21">
         <v>125</v>
       </c>
+      <c r="K21">
+        <v>202</v>
+      </c>
       <c r="M21">
         <v>9</v>
       </c>
       <c r="N21">
         <v>162</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
       <c r="B22">
         <v>173</v>
       </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22">
         <v>185</v>
       </c>
+      <c r="G22">
+        <v>98</v>
+      </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="J22">
         <v>131</v>
       </c>
+      <c r="K22">
+        <v>203</v>
+      </c>
       <c r="M22">
         <v>10</v>
       </c>
       <c r="N22">
         <v>183</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
       <c r="B23">
         <v>181</v>
       </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
       <c r="E23">
         <v>11</v>
       </c>
       <c r="F23">
         <v>189</v>
       </c>
+      <c r="G23">
+        <v>99</v>
+      </c>
       <c r="I23">
         <v>11</v>
       </c>
       <c r="J23">
         <v>147</v>
       </c>
+      <c r="K23">
+        <v>204</v>
+      </c>
       <c r="M23">
         <v>11</v>
       </c>
       <c r="N23">
         <v>196</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
       <c r="B24">
         <v>189</v>
       </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
       <c r="E24">
         <v>12</v>
       </c>
       <c r="F24">
         <v>203</v>
       </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
       <c r="I24">
         <v>12</v>
       </c>
       <c r="J24">
         <v>166</v>
       </c>
+      <c r="K24">
+        <v>205</v>
+      </c>
       <c r="M24">
         <v>12</v>
       </c>
       <c r="N24">
         <v>212</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25">
         <v>201</v>
       </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
       <c r="F25">
         <v>221</v>
       </c>
+      <c r="G25">
+        <v>101</v>
+      </c>
       <c r="I25">
         <v>13</v>
       </c>
       <c r="J25">
         <v>187</v>
       </c>
+      <c r="K25">
+        <v>206</v>
+      </c>
       <c r="M25">
         <v>13</v>
       </c>
       <c r="N25">
         <v>234</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26">
         <v>208</v>
       </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="F26">
         <v>233</v>
       </c>
+      <c r="G26">
+        <v>102</v>
+      </c>
       <c r="I26">
         <v>14</v>
       </c>
       <c r="J26">
         <v>200</v>
       </c>
+      <c r="K26">
+        <v>207</v>
+      </c>
       <c r="M26">
         <v>14</v>
       </c>
       <c r="N26">
         <v>255</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27">
         <v>213</v>
       </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27">
         <v>243</v>
       </c>
+      <c r="G27">
+        <v>103</v>
+      </c>
       <c r="I27">
         <v>15</v>
       </c>
       <c r="J27">
         <v>205</v>
       </c>
+      <c r="K27">
+        <v>208</v>
+      </c>
       <c r="M27">
         <v>15</v>
       </c>
       <c r="N27">
         <v>276</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
       <c r="B28">
         <v>221</v>
       </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
       <c r="E28" t="s">
         <v>13</v>
       </c>
       <c r="F28">
         <v>268</v>
       </c>
+      <c r="G28">
+        <v>104</v>
+      </c>
       <c r="I28">
         <v>16</v>
       </c>
       <c r="J28">
         <v>217</v>
       </c>
+      <c r="K28">
+        <v>209</v>
+      </c>
       <c r="M28">
         <v>16</v>
       </c>
       <c r="N28">
         <v>298</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>13</v>
       </c>
       <c r="B29">
         <v>245</v>
       </c>
+      <c r="C29">
+        <v>18</v>
+      </c>
       <c r="E29">
         <v>13</v>
       </c>
       <c r="F29">
         <v>283</v>
       </c>
+      <c r="G29">
+        <v>105</v>
+      </c>
       <c r="I29">
         <v>17</v>
       </c>
       <c r="J29">
         <v>239</v>
       </c>
+      <c r="K29">
+        <v>210</v>
+      </c>
       <c r="M29">
         <v>17</v>
       </c>
       <c r="N29">
         <v>315</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30">
         <v>256</v>
       </c>
+      <c r="C30">
+        <v>19</v>
+      </c>
       <c r="E30">
         <v>14</v>
       </c>
       <c r="F30">
         <v>294</v>
       </c>
+      <c r="G30">
+        <v>106</v>
+      </c>
       <c r="I30">
         <v>18</v>
       </c>
       <c r="J30">
         <v>250</v>
       </c>
+      <c r="K30">
+        <v>211</v>
+      </c>
       <c r="M30">
         <v>18</v>
       </c>
       <c r="N30">
         <v>332</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31">
         <v>268</v>
       </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
       <c r="E31">
         <v>15</v>
       </c>
       <c r="F31">
         <v>305</v>
       </c>
+      <c r="G31">
+        <v>107</v>
+      </c>
       <c r="I31">
         <v>19</v>
       </c>
       <c r="J31">
         <v>273</v>
       </c>
+      <c r="K31">
+        <v>212</v>
+      </c>
       <c r="M31">
         <v>19</v>
       </c>
       <c r="N31">
         <v>344</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>16</v>
       </c>
       <c r="B32">
         <v>297</v>
       </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
       <c r="E32">
         <v>16</v>
       </c>
       <c r="F32">
         <v>313</v>
       </c>
+      <c r="G32">
+        <v>108</v>
+      </c>
       <c r="I32">
         <v>20</v>
       </c>
       <c r="J32">
         <v>287</v>
       </c>
+      <c r="K32">
+        <v>213</v>
+      </c>
       <c r="M32" t="s">
         <v>10</v>
       </c>
       <c r="N32">
         <v>371</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>17</v>
       </c>
       <c r="B33">
         <v>314</v>
       </c>
+      <c r="C33">
+        <v>22</v>
+      </c>
       <c r="E33">
         <v>17</v>
       </c>
       <c r="F33">
         <v>330</v>
       </c>
+      <c r="G33">
+        <v>109</v>
+      </c>
       <c r="I33">
         <v>21</v>
       </c>
       <c r="J33">
         <v>292</v>
       </c>
+      <c r="K33">
+        <v>214</v>
+      </c>
       <c r="M33" t="s">
         <v>11</v>
       </c>
       <c r="N33">
         <v>381</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>18</v>
       </c>
       <c r="B34">
         <v>345</v>
       </c>
+      <c r="C34">
+        <v>23</v>
+      </c>
       <c r="E34">
         <v>18</v>
       </c>
       <c r="F34">
         <v>347</v>
       </c>
+      <c r="G34">
+        <v>110</v>
+      </c>
       <c r="I34">
         <v>22</v>
       </c>
       <c r="J34">
         <v>305</v>
       </c>
+      <c r="K34">
+        <v>215</v>
+      </c>
       <c r="M34" t="s">
         <v>12</v>
       </c>
       <c r="N34">
         <v>387</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>19</v>
       </c>
       <c r="B35">
         <v>361</v>
       </c>
+      <c r="C35">
+        <v>24</v>
+      </c>
       <c r="E35">
         <v>19</v>
       </c>
       <c r="F35">
         <v>361</v>
       </c>
+      <c r="G35">
+        <v>111</v>
+      </c>
       <c r="I35">
         <v>23</v>
       </c>
       <c r="J35">
         <v>313</v>
       </c>
+      <c r="K35">
+        <v>216</v>
+      </c>
       <c r="M35">
         <v>20</v>
       </c>
       <c r="N35">
         <v>395</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20</v>
       </c>
       <c r="B36">
         <v>379</v>
       </c>
+      <c r="C36">
+        <v>25</v>
+      </c>
       <c r="E36">
         <v>20</v>
       </c>
       <c r="F36">
         <v>366</v>
       </c>
+      <c r="G36">
+        <v>112</v>
+      </c>
       <c r="I36">
         <v>24</v>
       </c>
       <c r="J36">
         <v>319</v>
       </c>
+      <c r="K36">
+        <v>217</v>
+      </c>
       <c r="M36">
         <v>21</v>
       </c>
       <c r="N36">
         <v>407</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>21</v>
       </c>
       <c r="B37">
         <v>382</v>
       </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
       <c r="E37">
         <v>21</v>
       </c>
       <c r="F37">
         <v>376</v>
       </c>
+      <c r="G37">
+        <v>113</v>
+      </c>
       <c r="I37">
         <v>25</v>
       </c>
       <c r="J37">
         <v>334</v>
       </c>
+      <c r="K37">
+        <v>218</v>
+      </c>
       <c r="M37">
         <v>22</v>
       </c>
       <c r="N37">
         <v>429</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>22</v>
       </c>
       <c r="B38">
         <v>396</v>
       </c>
+      <c r="C38">
+        <v>27</v>
+      </c>
       <c r="E38">
         <v>22</v>
       </c>
       <c r="F38">
         <v>386</v>
       </c>
+      <c r="G38">
+        <v>114</v>
+      </c>
       <c r="I38">
         <v>26</v>
       </c>
       <c r="J38">
         <v>347</v>
       </c>
+      <c r="K38">
+        <v>219</v>
+      </c>
       <c r="M38">
         <v>23</v>
       </c>
       <c r="N38">
         <v>447</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>23</v>
       </c>
       <c r="B39">
         <v>414</v>
       </c>
+      <c r="C39">
+        <v>28</v>
+      </c>
       <c r="E39">
         <v>23</v>
       </c>
       <c r="F39">
         <v>402</v>
       </c>
+      <c r="G39">
+        <v>115</v>
+      </c>
       <c r="I39">
         <v>27</v>
       </c>
       <c r="J39">
         <v>365</v>
       </c>
+      <c r="K39">
+        <v>220</v>
+      </c>
       <c r="M39">
         <v>24</v>
       </c>
       <c r="N39">
         <v>458</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>24</v>
       </c>
       <c r="B40">
         <v>432</v>
       </c>
+      <c r="C40">
+        <v>29</v>
+      </c>
       <c r="E40">
         <v>24</v>
       </c>
       <c r="F40">
         <v>409</v>
       </c>
+      <c r="G40">
+        <v>116</v>
+      </c>
       <c r="I40">
         <v>28</v>
       </c>
       <c r="J40">
         <v>378</v>
       </c>
+      <c r="K40">
+        <v>221</v>
+      </c>
       <c r="M40">
         <v>25</v>
       </c>
       <c r="N40">
         <v>469</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>25</v>
       </c>
       <c r="B41">
         <v>444</v>
       </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
       <c r="E41">
         <v>25</v>
       </c>
       <c r="F41">
         <v>424</v>
       </c>
+      <c r="G41">
+        <v>117</v>
+      </c>
       <c r="I41">
         <v>29</v>
       </c>
       <c r="J41">
         <v>393</v>
       </c>
+      <c r="K41">
+        <v>222</v>
+      </c>
       <c r="M41">
         <v>26</v>
       </c>
       <c r="N41">
         <v>483</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>26</v>
       </c>
       <c r="B42">
         <v>454</v>
       </c>
+      <c r="C42">
+        <v>31</v>
+      </c>
       <c r="E42">
         <v>26</v>
       </c>
       <c r="F42">
         <v>440</v>
       </c>
+      <c r="G42">
+        <v>118</v>
+      </c>
       <c r="I42">
         <v>30</v>
       </c>
       <c r="J42">
         <v>415</v>
       </c>
+      <c r="K42">
+        <v>223</v>
+      </c>
       <c r="M42">
         <v>27</v>
       </c>
       <c r="N42">
         <v>508</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>27</v>
       </c>
       <c r="B43">
         <v>474</v>
       </c>
+      <c r="C43">
+        <v>32</v>
+      </c>
       <c r="E43">
         <v>27</v>
       </c>
       <c r="F43">
         <v>454</v>
       </c>
+      <c r="G43">
+        <v>119</v>
+      </c>
       <c r="I43">
         <v>31</v>
       </c>
       <c r="J43">
         <v>419</v>
       </c>
+      <c r="K43">
+        <v>224</v>
+      </c>
       <c r="M43">
         <v>28</v>
       </c>
       <c r="N43">
         <v>521</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>28</v>
       </c>
       <c r="B44">
         <v>501</v>
       </c>
+      <c r="C44">
+        <v>33</v>
+      </c>
       <c r="E44">
         <v>28</v>
       </c>
       <c r="F44">
         <v>458</v>
       </c>
+      <c r="G44">
+        <v>120</v>
+      </c>
       <c r="I44">
         <v>32</v>
       </c>
       <c r="J44">
         <v>436</v>
       </c>
+      <c r="K44">
+        <v>225</v>
+      </c>
       <c r="M44">
         <v>29</v>
       </c>
       <c r="N44">
         <v>528</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45">
         <v>532</v>
       </c>
+      <c r="C45">
+        <v>34</v>
+      </c>
       <c r="E45">
         <v>29</v>
       </c>
       <c r="F45">
         <v>469</v>
       </c>
+      <c r="G45">
+        <v>121</v>
+      </c>
       <c r="I45" t="s">
         <v>10</v>
       </c>
       <c r="J45">
         <v>442</v>
       </c>
+      <c r="K45">
+        <v>226</v>
+      </c>
       <c r="M45">
         <v>30</v>
       </c>
       <c r="N45">
         <v>545</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
       <c r="B46">
         <v>541</v>
       </c>
+      <c r="C46">
+        <v>35</v>
+      </c>
       <c r="E46">
         <v>30</v>
       </c>
       <c r="F46">
         <v>481</v>
       </c>
+      <c r="G46">
+        <v>122</v>
+      </c>
       <c r="I46" t="s">
         <v>11</v>
       </c>
       <c r="J46">
         <v>445</v>
       </c>
+      <c r="K46">
+        <v>227</v>
+      </c>
       <c r="M46">
         <v>31</v>
       </c>
       <c r="N46">
         <v>560</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
       <c r="B47">
         <v>548</v>
       </c>
+      <c r="C47">
+        <v>36</v>
+      </c>
       <c r="E47">
         <v>31</v>
       </c>
       <c r="F47">
         <v>491</v>
       </c>
+      <c r="G47">
+        <v>123</v>
+      </c>
       <c r="I47" t="s">
         <v>12</v>
       </c>
       <c r="J47">
         <v>452</v>
       </c>
+      <c r="K47">
+        <v>228</v>
+      </c>
       <c r="M47">
         <v>32</v>
       </c>
       <c r="N47">
         <v>568</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>29</v>
       </c>
       <c r="B48">
         <v>560</v>
       </c>
+      <c r="C48">
+        <v>37</v>
+      </c>
       <c r="E48">
         <v>32</v>
       </c>
       <c r="F48">
         <v>500</v>
       </c>
+      <c r="G48">
+        <v>124</v>
+      </c>
       <c r="I48">
         <v>33</v>
       </c>
       <c r="J48">
         <v>461</v>
       </c>
+      <c r="K48">
+        <v>229</v>
+      </c>
       <c r="M48">
         <v>33</v>
       </c>
       <c r="N48">
         <v>578</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>30</v>
       </c>
       <c r="B49">
         <v>581</v>
       </c>
+      <c r="C49">
+        <v>38</v>
+      </c>
       <c r="E49">
         <v>33</v>
       </c>
       <c r="F49">
         <v>513</v>
       </c>
+      <c r="G49">
+        <v>125</v>
+      </c>
       <c r="I49">
         <v>34</v>
       </c>
       <c r="J49">
         <v>468</v>
       </c>
+      <c r="K49">
+        <v>230</v>
+      </c>
       <c r="M49">
         <v>34</v>
       </c>
       <c r="N49">
         <v>581</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>31</v>
       </c>
       <c r="B50">
         <v>593</v>
       </c>
+      <c r="C50">
+        <v>39</v>
+      </c>
       <c r="E50">
         <v>34</v>
       </c>
       <c r="F50">
         <v>524</v>
       </c>
+      <c r="G50">
+        <v>126</v>
+      </c>
       <c r="I50">
         <v>35</v>
       </c>
       <c r="J50">
         <v>484</v>
       </c>
+      <c r="K50">
+        <v>231</v>
+      </c>
       <c r="M50">
         <v>35</v>
       </c>
       <c r="N50">
         <v>598</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>32</v>
       </c>
       <c r="B51">
         <v>600</v>
       </c>
+      <c r="C51">
+        <v>40</v>
+      </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
       <c r="F51">
         <v>536</v>
       </c>
+      <c r="G51">
+        <v>127</v>
+      </c>
       <c r="I51">
         <v>36</v>
       </c>
       <c r="J51">
         <v>498</v>
       </c>
+      <c r="K51">
+        <v>232</v>
+      </c>
       <c r="M51">
         <v>36</v>
       </c>
       <c r="N51">
         <v>615</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>33</v>
       </c>
       <c r="B52">
         <v>616</v>
       </c>
+      <c r="C52">
+        <v>41</v>
+      </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="F52">
         <v>541</v>
       </c>
+      <c r="G52">
+        <v>128</v>
+      </c>
       <c r="I52">
         <v>37</v>
       </c>
       <c r="J52">
         <v>505</v>
       </c>
+      <c r="K52">
+        <v>233</v>
+      </c>
       <c r="M52">
         <v>37</v>
       </c>
       <c r="N52">
         <v>629</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>34</v>
       </c>
       <c r="B53">
         <v>634</v>
       </c>
+      <c r="C53">
+        <v>42</v>
+      </c>
       <c r="E53" t="s">
         <v>16</v>
       </c>
       <c r="F53">
         <v>543</v>
       </c>
+      <c r="G53">
+        <v>129</v>
+      </c>
       <c r="I53">
         <v>38</v>
       </c>
       <c r="J53">
         <v>530</v>
       </c>
+      <c r="K53">
+        <v>234</v>
+      </c>
       <c r="M53">
         <v>38</v>
       </c>
       <c r="N53">
         <v>646</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>35</v>
       </c>
       <c r="B54">
         <v>641</v>
       </c>
+      <c r="C54">
+        <v>43</v>
+      </c>
       <c r="E54" t="s">
         <v>17</v>
       </c>
       <c r="F54">
         <v>547</v>
       </c>
+      <c r="G54">
+        <v>130</v>
+      </c>
       <c r="I54">
         <v>39</v>
       </c>
       <c r="J54">
         <v>550</v>
       </c>
+      <c r="K54">
+        <v>235</v>
+      </c>
       <c r="M54">
         <v>39</v>
       </c>
       <c r="N54">
         <v>657</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>36</v>
       </c>
       <c r="B55">
         <v>647</v>
       </c>
+      <c r="C55">
+        <v>44</v>
+      </c>
       <c r="E55">
         <v>35</v>
       </c>
       <c r="F55">
         <v>552</v>
       </c>
+      <c r="G55">
+        <v>131</v>
+      </c>
       <c r="I55">
         <v>40</v>
       </c>
       <c r="J55">
         <v>563</v>
       </c>
+      <c r="K55">
+        <v>236</v>
+      </c>
       <c r="M55">
         <v>40</v>
       </c>
       <c r="N55">
         <v>675</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>37</v>
       </c>
       <c r="B56">
         <v>665</v>
       </c>
+      <c r="C56">
+        <v>45</v>
+      </c>
       <c r="E56">
         <v>36</v>
       </c>
       <c r="F56">
         <v>568</v>
       </c>
+      <c r="G56">
+        <v>132</v>
+      </c>
       <c r="I56">
         <v>41</v>
       </c>
       <c r="J56">
         <v>575</v>
       </c>
+      <c r="K56">
+        <v>237</v>
+      </c>
       <c r="M56">
         <v>41</v>
       </c>
       <c r="N56">
         <v>686</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>38</v>
       </c>
       <c r="B57">
         <v>683</v>
       </c>
+      <c r="C57">
+        <v>46</v>
+      </c>
       <c r="E57">
         <v>37</v>
       </c>
       <c r="F57">
         <v>584</v>
       </c>
+      <c r="G57">
+        <v>133</v>
+      </c>
       <c r="I57">
         <v>42</v>
       </c>
       <c r="J57">
         <v>582</v>
       </c>
+      <c r="K57">
+        <v>238</v>
+      </c>
       <c r="M57">
         <v>42</v>
       </c>
       <c r="N57">
         <v>699</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>39</v>
       </c>
       <c r="B58">
         <v>689</v>
       </c>
+      <c r="C58">
+        <v>47</v>
+      </c>
       <c r="E58">
         <v>38</v>
       </c>
       <c r="F58">
         <v>594</v>
       </c>
+      <c r="G58">
+        <v>134</v>
+      </c>
       <c r="I58">
         <v>43</v>
       </c>
       <c r="J58">
         <v>590</v>
       </c>
+      <c r="K58">
+        <v>239</v>
+      </c>
       <c r="M58">
         <v>43</v>
       </c>
       <c r="N58">
         <v>722</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>40</v>
       </c>
       <c r="B59">
         <v>701</v>
       </c>
+      <c r="C59">
+        <v>48</v>
+      </c>
       <c r="E59">
         <v>39</v>
       </c>
       <c r="F59">
         <v>612</v>
       </c>
+      <c r="G59">
+        <v>135</v>
+      </c>
       <c r="I59">
         <v>44</v>
       </c>
       <c r="J59">
         <v>599</v>
       </c>
+      <c r="K59">
+        <v>240</v>
+      </c>
       <c r="M59" t="s">
         <v>13</v>
       </c>
       <c r="N59">
         <v>739</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>41</v>
       </c>
       <c r="B60">
         <v>718</v>
       </c>
+      <c r="C60">
+        <v>49</v>
+      </c>
       <c r="E60">
         <v>40</v>
       </c>
       <c r="F60">
         <v>623</v>
       </c>
+      <c r="G60">
+        <v>136</v>
+      </c>
       <c r="I60">
         <v>45</v>
       </c>
       <c r="J60">
         <v>614</v>
       </c>
+      <c r="K60">
+        <v>241</v>
+      </c>
       <c r="M60" t="s">
         <v>14</v>
       </c>
       <c r="N60">
         <v>748</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>42</v>
       </c>
       <c r="B61">
         <v>725</v>
       </c>
+      <c r="C61">
+        <v>50</v>
+      </c>
       <c r="E61">
         <v>41</v>
       </c>
       <c r="F61">
         <v>631</v>
       </c>
+      <c r="G61">
+        <v>137</v>
+      </c>
       <c r="I61">
         <v>46</v>
       </c>
       <c r="J61">
         <v>623</v>
       </c>
+      <c r="K61">
+        <v>242</v>
+      </c>
       <c r="M61" t="s">
         <v>15</v>
       </c>
       <c r="N61">
         <v>762</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>43</v>
       </c>
       <c r="B62">
         <v>742</v>
       </c>
+      <c r="C62">
+        <v>51</v>
+      </c>
       <c r="E62">
         <v>42</v>
       </c>
       <c r="F62">
         <v>640</v>
       </c>
+      <c r="G62">
+        <v>138</v>
+      </c>
       <c r="I62">
         <v>47</v>
       </c>
       <c r="J62">
         <v>638</v>
       </c>
+      <c r="K62">
+        <v>243</v>
+      </c>
       <c r="M62">
         <v>44</v>
       </c>
       <c r="N62">
         <v>774</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>44</v>
       </c>
       <c r="B63">
         <v>758</v>
       </c>
+      <c r="C63">
+        <v>52</v>
+      </c>
       <c r="E63">
         <v>43</v>
       </c>
       <c r="F63">
         <v>659</v>
       </c>
+      <c r="G63">
+        <v>139</v>
+      </c>
       <c r="I63">
         <v>48</v>
       </c>
       <c r="J63">
         <v>645</v>
       </c>
+      <c r="K63">
+        <v>244</v>
+      </c>
       <c r="M63">
         <v>45</v>
       </c>
       <c r="N63">
         <v>784</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>45</v>
       </c>
       <c r="B64">
         <v>773</v>
       </c>
+      <c r="C64">
+        <v>53</v>
+      </c>
       <c r="E64">
         <v>44</v>
       </c>
       <c r="F64">
         <v>677</v>
       </c>
+      <c r="G64">
+        <v>140</v>
+      </c>
       <c r="I64">
         <v>49</v>
       </c>
       <c r="J64">
         <v>652</v>
       </c>
+      <c r="K64">
+        <v>245</v>
+      </c>
       <c r="M64">
         <v>46</v>
       </c>
       <c r="N64">
         <v>794</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>46</v>
       </c>
       <c r="B65">
         <v>797</v>
       </c>
+      <c r="C65">
+        <v>54</v>
+      </c>
       <c r="E65">
         <v>45</v>
       </c>
       <c r="F65">
         <v>697</v>
       </c>
+      <c r="G65">
+        <v>141</v>
+      </c>
       <c r="I65">
         <v>50</v>
       </c>
       <c r="J65">
         <v>667</v>
       </c>
+      <c r="K65">
+        <v>246</v>
+      </c>
       <c r="M65">
         <v>47</v>
       </c>
       <c r="N65">
         <v>808</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>47</v>
       </c>
       <c r="B66">
         <v>819</v>
       </c>
+      <c r="C66">
+        <v>55</v>
+      </c>
       <c r="E66">
         <v>46</v>
       </c>
       <c r="F66">
         <v>719</v>
       </c>
+      <c r="G66">
+        <v>142</v>
+      </c>
       <c r="I66">
         <v>51</v>
       </c>
       <c r="J66">
         <v>680</v>
       </c>
+      <c r="K66">
+        <v>247</v>
+      </c>
       <c r="M66">
         <v>48</v>
       </c>
       <c r="N66">
         <v>819</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>48</v>
       </c>
       <c r="B67">
         <v>836</v>
       </c>
+      <c r="C67">
+        <v>56</v>
+      </c>
       <c r="E67">
         <v>47</v>
       </c>
       <c r="F67">
         <v>742</v>
       </c>
+      <c r="G67">
+        <v>143</v>
+      </c>
       <c r="I67">
         <v>52</v>
       </c>
       <c r="J67">
         <v>689</v>
       </c>
+      <c r="K67">
+        <v>248</v>
+      </c>
       <c r="M67">
         <v>49</v>
       </c>
       <c r="N67">
         <v>827</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>49</v>
       </c>
       <c r="B68">
         <v>848</v>
       </c>
+      <c r="C68">
+        <v>57</v>
+      </c>
       <c r="E68">
         <v>48</v>
       </c>
       <c r="F68">
         <v>754</v>
       </c>
+      <c r="G68">
+        <v>144</v>
+      </c>
       <c r="I68">
         <v>53</v>
       </c>
       <c r="J68">
         <v>699</v>
       </c>
+      <c r="K68">
+        <v>249</v>
+      </c>
       <c r="M68">
         <v>50</v>
       </c>
       <c r="N68">
         <v>847</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>50</v>
       </c>
       <c r="B69">
         <v>859</v>
       </c>
+      <c r="C69">
+        <v>58</v>
+      </c>
       <c r="E69">
         <v>49</v>
       </c>
       <c r="F69">
         <v>768</v>
       </c>
+      <c r="G69">
+        <v>145</v>
+      </c>
       <c r="I69">
         <v>54</v>
       </c>
       <c r="J69">
         <v>712</v>
       </c>
+      <c r="K69">
+        <v>250</v>
+      </c>
       <c r="M69">
         <v>51</v>
       </c>
       <c r="N69">
         <v>867</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>51</v>
       </c>
       <c r="B70">
         <v>864</v>
       </c>
+      <c r="C70">
+        <v>59</v>
+      </c>
       <c r="E70">
         <v>50</v>
       </c>
       <c r="F70">
         <v>790</v>
       </c>
+      <c r="G70">
+        <v>146</v>
+      </c>
       <c r="I70">
         <v>55</v>
       </c>
       <c r="J70">
         <v>722</v>
       </c>
+      <c r="K70">
+        <v>251</v>
+      </c>
       <c r="M70">
         <v>52</v>
       </c>
       <c r="N70">
         <v>874</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O70">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B71">
         <v>872</v>
       </c>
+      <c r="C71">
+        <v>60</v>
+      </c>
       <c r="E71">
         <v>51</v>
       </c>
       <c r="F71">
         <v>800</v>
       </c>
+      <c r="G71">
+        <v>147</v>
+      </c>
       <c r="I71">
         <v>56</v>
       </c>
       <c r="J71">
         <v>732</v>
       </c>
+      <c r="K71">
+        <v>252</v>
+      </c>
       <c r="M71">
         <v>53</v>
       </c>
       <c r="N71">
         <v>883</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O71">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B72">
         <v>877</v>
       </c>
+      <c r="C72">
+        <v>61</v>
+      </c>
       <c r="E72">
         <v>52</v>
       </c>
       <c r="F72">
         <v>810</v>
       </c>
+      <c r="G72">
+        <v>148</v>
+      </c>
       <c r="I72">
         <v>57</v>
       </c>
       <c r="J72">
         <v>740</v>
       </c>
+      <c r="K72">
+        <v>253</v>
+      </c>
       <c r="M72">
         <v>54</v>
       </c>
       <c r="N72">
         <v>892</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O72">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B73">
         <v>882</v>
       </c>
+      <c r="C73">
+        <v>62</v>
+      </c>
       <c r="E73">
         <v>53</v>
       </c>
       <c r="F73">
         <v>837</v>
       </c>
+      <c r="G73">
+        <v>149</v>
+      </c>
       <c r="I73" t="s">
         <v>13</v>
       </c>
       <c r="J73">
         <v>749</v>
       </c>
+      <c r="K73">
+        <v>254</v>
+      </c>
       <c r="M73">
         <v>55</v>
       </c>
       <c r="N73">
         <v>903</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>52</v>
       </c>
       <c r="B74">
         <v>892</v>
       </c>
+      <c r="C74">
+        <v>63</v>
+      </c>
       <c r="E74">
         <v>54</v>
       </c>
       <c r="F74">
         <v>847</v>
       </c>
+      <c r="G74">
+        <v>150</v>
+      </c>
       <c r="I74" t="s">
         <v>14</v>
       </c>
       <c r="J74">
         <v>760</v>
       </c>
+      <c r="K74">
+        <v>255</v>
+      </c>
       <c r="M74">
         <v>56</v>
       </c>
       <c r="N74">
         <v>914</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>53</v>
       </c>
       <c r="B75">
         <v>913</v>
       </c>
+      <c r="C75">
+        <v>64</v>
+      </c>
       <c r="E75">
         <v>55</v>
       </c>
       <c r="F75">
         <v>862</v>
       </c>
+      <c r="G75">
+        <v>151</v>
+      </c>
       <c r="I75" t="s">
         <v>15</v>
       </c>
       <c r="J75">
         <v>771</v>
       </c>
+      <c r="K75">
+        <v>256</v>
+      </c>
       <c r="M75">
         <v>57</v>
       </c>
       <c r="N75">
         <v>924</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O75">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>54</v>
       </c>
       <c r="B76">
         <v>922</v>
       </c>
+      <c r="C76">
+        <v>65</v>
+      </c>
       <c r="E76">
         <v>56</v>
       </c>
       <c r="F76">
         <v>883</v>
       </c>
+      <c r="G76">
+        <v>152</v>
+      </c>
       <c r="I76">
         <v>58</v>
       </c>
       <c r="J76">
         <v>781</v>
       </c>
+      <c r="K76">
+        <v>257</v>
+      </c>
       <c r="M76">
         <v>58</v>
       </c>
       <c r="N76">
         <v>936</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O76">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>55</v>
       </c>
       <c r="B77">
         <v>940</v>
       </c>
+      <c r="C77">
+        <v>66</v>
+      </c>
       <c r="E77">
         <v>57</v>
       </c>
       <c r="F77">
         <v>900</v>
       </c>
+      <c r="G77">
+        <v>153</v>
+      </c>
       <c r="I77">
         <v>59</v>
       </c>
       <c r="J77">
         <v>789</v>
       </c>
+      <c r="K77">
+        <v>258</v>
+      </c>
       <c r="M77">
         <v>59</v>
       </c>
       <c r="N77">
         <v>945</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O77">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>56</v>
       </c>
       <c r="B78">
         <v>958</v>
       </c>
+      <c r="C78">
+        <v>67</v>
+      </c>
       <c r="E78">
         <v>58</v>
       </c>
       <c r="F78">
         <v>914</v>
       </c>
+      <c r="G78">
+        <v>154</v>
+      </c>
       <c r="I78">
         <v>60</v>
       </c>
       <c r="J78">
         <v>807</v>
       </c>
+      <c r="K78">
+        <v>259</v>
+      </c>
       <c r="M78">
         <v>60</v>
       </c>
       <c r="N78">
         <v>963</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O78">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>57</v>
       </c>
       <c r="B79">
         <v>974</v>
       </c>
+      <c r="C79">
+        <v>68</v>
+      </c>
       <c r="E79" t="s">
         <v>18</v>
       </c>
       <c r="F79">
         <v>923</v>
       </c>
+      <c r="G79">
+        <v>155</v>
+      </c>
       <c r="I79">
         <v>61</v>
       </c>
       <c r="J79">
         <v>817</v>
       </c>
+      <c r="K79">
+        <v>260</v>
+      </c>
       <c r="M79">
         <v>61</v>
       </c>
       <c r="N79">
         <v>976</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O79">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>58</v>
       </c>
       <c r="B80">
         <v>1001</v>
       </c>
+      <c r="C80">
+        <v>69</v>
+      </c>
       <c r="E80" t="s">
         <v>22</v>
       </c>
       <c r="F80">
         <v>959</v>
       </c>
+      <c r="G80">
+        <v>156</v>
+      </c>
       <c r="I80">
         <v>62</v>
       </c>
       <c r="J80">
         <v>833</v>
       </c>
+      <c r="K80">
+        <v>261</v>
+      </c>
       <c r="M80">
         <v>62</v>
       </c>
       <c r="N80">
         <v>990</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O80">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>59</v>
       </c>
       <c r="B81">
         <v>1023</v>
       </c>
+      <c r="C81">
+        <v>70</v>
+      </c>
       <c r="E81" t="s">
         <v>23</v>
       </c>
       <c r="F81">
         <v>962</v>
       </c>
+      <c r="G81">
+        <v>157</v>
+      </c>
       <c r="I81">
         <v>63</v>
       </c>
       <c r="J81">
         <v>847</v>
       </c>
+      <c r="K81">
+        <v>262</v>
+      </c>
       <c r="M81">
         <v>63</v>
       </c>
       <c r="N81">
         <v>997</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O81">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>60</v>
       </c>
       <c r="B82">
         <v>1043</v>
       </c>
+      <c r="C82">
+        <v>71</v>
+      </c>
       <c r="E82">
         <v>59</v>
       </c>
       <c r="F82">
         <v>979</v>
       </c>
+      <c r="G82">
+        <v>158</v>
+      </c>
       <c r="I82">
         <v>64</v>
       </c>
       <c r="J82">
         <v>858</v>
       </c>
+      <c r="K82">
+        <v>263</v>
+      </c>
       <c r="M82">
         <v>64</v>
       </c>
       <c r="N82">
         <v>1010</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O82">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>61</v>
       </c>
       <c r="B83">
         <v>1057</v>
       </c>
+      <c r="C83">
+        <v>72</v>
+      </c>
       <c r="E83">
         <v>60</v>
       </c>
       <c r="F83">
         <v>990</v>
       </c>
+      <c r="G83">
+        <v>159</v>
+      </c>
       <c r="I83">
         <v>65</v>
       </c>
       <c r="J83">
         <v>869</v>
       </c>
+      <c r="K83">
+        <v>264</v>
+      </c>
       <c r="M83">
         <v>65</v>
       </c>
       <c r="N83">
         <v>1025</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O83">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>62</v>
       </c>
       <c r="B84">
         <v>1068</v>
       </c>
+      <c r="C84">
+        <v>73</v>
+      </c>
       <c r="E84">
         <v>61</v>
       </c>
       <c r="F84">
         <v>1001</v>
       </c>
+      <c r="G84">
+        <v>160</v>
+      </c>
       <c r="I84">
         <v>66</v>
       </c>
       <c r="J84">
         <v>886</v>
       </c>
+      <c r="K84">
+        <v>265</v>
+      </c>
       <c r="M84">
         <v>66</v>
       </c>
       <c r="N84">
         <v>1033</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O84">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>63</v>
       </c>
       <c r="B85">
         <v>1084</v>
       </c>
+      <c r="C85">
+        <v>74</v>
+      </c>
       <c r="E85">
         <v>62</v>
       </c>
       <c r="F85">
         <v>1008</v>
       </c>
+      <c r="G85">
+        <v>161</v>
+      </c>
       <c r="I85">
         <v>67</v>
       </c>
       <c r="J85">
         <v>897</v>
       </c>
+      <c r="K85">
+        <v>266</v>
+      </c>
       <c r="M85">
         <v>67</v>
       </c>
       <c r="N85">
         <v>1045</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O85">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>64</v>
       </c>
       <c r="B86">
         <v>1091</v>
       </c>
+      <c r="C86">
+        <v>75</v>
+      </c>
       <c r="E86">
         <v>63</v>
       </c>
       <c r="F86">
         <v>1016</v>
       </c>
+      <c r="G86">
+        <v>162</v>
+      </c>
       <c r="I86">
         <v>68</v>
       </c>
       <c r="J86">
         <v>912</v>
       </c>
+      <c r="K86">
+        <v>267</v>
+      </c>
       <c r="M86">
         <v>68</v>
       </c>
       <c r="N86">
         <v>1053</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>65</v>
       </c>
       <c r="B87">
         <v>1102</v>
       </c>
+      <c r="C87">
+        <v>76</v>
+      </c>
       <c r="E87">
         <v>64</v>
       </c>
       <c r="F87">
         <v>1035</v>
       </c>
+      <c r="G87">
+        <v>163</v>
+      </c>
       <c r="I87">
         <v>69</v>
       </c>
       <c r="J87">
         <v>924</v>
       </c>
+      <c r="K87">
+        <v>268</v>
+      </c>
       <c r="M87">
         <v>69</v>
       </c>
       <c r="N87">
         <v>1065</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O87">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>66</v>
       </c>
       <c r="B88">
         <v>1114</v>
       </c>
+      <c r="C88">
+        <v>77</v>
+      </c>
       <c r="E88">
         <v>65</v>
       </c>
       <c r="F88">
         <v>1042</v>
       </c>
+      <c r="G88">
+        <v>164</v>
+      </c>
       <c r="I88">
         <v>70</v>
       </c>
       <c r="J88">
         <v>934</v>
       </c>
+      <c r="K88">
+        <v>269</v>
+      </c>
       <c r="M88">
         <v>70</v>
       </c>
       <c r="N88">
         <v>1079</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O88">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>67</v>
       </c>
       <c r="B89">
         <v>1122</v>
       </c>
+      <c r="C89">
+        <v>78</v>
+      </c>
       <c r="E89">
         <v>66</v>
       </c>
       <c r="F89">
         <v>1049</v>
       </c>
+      <c r="G89">
+        <v>165</v>
+      </c>
       <c r="I89">
         <v>71</v>
       </c>
       <c r="J89">
         <v>943</v>
       </c>
+      <c r="K89">
+        <v>270</v>
+      </c>
       <c r="M89">
         <v>71</v>
       </c>
       <c r="N89">
         <v>1099</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O89">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>68</v>
       </c>
       <c r="B90">
         <v>1145</v>
       </c>
+      <c r="C90">
+        <v>79</v>
+      </c>
       <c r="E90">
         <v>67</v>
       </c>
       <c r="F90">
         <v>1060</v>
       </c>
+      <c r="G90">
+        <v>166</v>
+      </c>
       <c r="I90">
         <v>72</v>
       </c>
       <c r="J90">
         <v>955</v>
       </c>
+      <c r="K90">
+        <v>271</v>
+      </c>
       <c r="M90">
         <v>72</v>
       </c>
       <c r="N90">
         <v>1111</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O90">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>69</v>
       </c>
       <c r="B91">
         <v>1169</v>
       </c>
+      <c r="C91">
+        <v>80</v>
+      </c>
       <c r="E91">
         <v>68</v>
       </c>
       <c r="F91">
         <v>1081</v>
       </c>
+      <c r="G91">
+        <v>167</v>
+      </c>
       <c r="I91">
         <v>73</v>
       </c>
       <c r="J91">
         <v>969</v>
       </c>
+      <c r="K91">
+        <v>272</v>
+      </c>
       <c r="M91" t="s">
         <v>16</v>
       </c>
       <c r="N91">
         <v>1116</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O91">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>70</v>
       </c>
       <c r="B92">
         <v>1194</v>
       </c>
+      <c r="C92">
+        <v>81</v>
+      </c>
       <c r="E92">
         <v>69</v>
       </c>
       <c r="F92">
         <v>1105</v>
       </c>
+      <c r="G92">
+        <v>168</v>
+      </c>
       <c r="I92">
         <v>74</v>
       </c>
       <c r="J92">
         <v>982</v>
       </c>
+      <c r="K92">
+        <v>273</v>
+      </c>
       <c r="M92" t="s">
         <v>17</v>
       </c>
       <c r="N92">
         <v>1123</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O92">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>71</v>
       </c>
       <c r="B93">
         <v>1202</v>
       </c>
+      <c r="C93">
+        <v>82</v>
+      </c>
       <c r="E93">
         <v>70</v>
       </c>
       <c r="F93">
         <v>1120</v>
       </c>
+      <c r="G93">
+        <v>169</v>
+      </c>
       <c r="I93">
         <v>75</v>
       </c>
       <c r="J93">
         <v>992</v>
       </c>
+      <c r="K93">
+        <v>274</v>
+      </c>
       <c r="M93" t="s">
         <v>18</v>
       </c>
       <c r="N93">
         <v>1127</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O93">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>72</v>
       </c>
       <c r="B94">
         <v>1210</v>
       </c>
+      <c r="C94">
+        <v>83</v>
+      </c>
       <c r="E94">
         <v>71</v>
       </c>
       <c r="F94">
         <v>1137</v>
       </c>
+      <c r="G94">
+        <v>170</v>
+      </c>
       <c r="I94">
         <v>76</v>
       </c>
       <c r="J94">
         <v>1002</v>
       </c>
+      <c r="K94">
+        <v>275</v>
+      </c>
       <c r="M94">
         <v>73</v>
       </c>
       <c r="N94">
         <v>1135</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O94">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>73</v>
       </c>
       <c r="B95">
         <v>1214</v>
       </c>
+      <c r="C95">
+        <v>84</v>
+      </c>
       <c r="E95">
         <v>72</v>
       </c>
       <c r="F95">
         <v>1158</v>
       </c>
+      <c r="G95">
+        <v>171</v>
+      </c>
       <c r="I95">
         <v>77</v>
       </c>
       <c r="J95">
         <v>1015</v>
       </c>
+      <c r="K95">
+        <v>276</v>
+      </c>
       <c r="M95">
         <v>74</v>
       </c>
       <c r="N95">
         <v>1144</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O95">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>74</v>
       </c>
       <c r="B96">
         <v>1225</v>
       </c>
+      <c r="C96">
+        <v>85</v>
+      </c>
       <c r="E96">
         <v>73</v>
       </c>
       <c r="F96">
         <v>1172</v>
       </c>
+      <c r="G96">
+        <v>172</v>
+      </c>
       <c r="I96">
         <v>78</v>
       </c>
       <c r="J96">
         <v>1030</v>
       </c>
+      <c r="K96">
+        <v>277</v>
+      </c>
       <c r="M96">
         <v>75</v>
       </c>
       <c r="N96">
         <v>1153</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O96">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>75</v>
       </c>
       <c r="B97">
         <v>1229</v>
       </c>
+      <c r="C97">
+        <v>86</v>
+      </c>
       <c r="E97">
         <v>74</v>
       </c>
       <c r="F97">
         <v>1183</v>
       </c>
+      <c r="G97">
+        <v>173</v>
+      </c>
       <c r="I97">
         <v>79</v>
       </c>
       <c r="J97">
         <v>1043</v>
       </c>
+      <c r="K97">
+        <v>278</v>
+      </c>
       <c r="M97">
         <v>76</v>
       </c>
       <c r="N97">
         <v>1169</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O97">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>19</v>
       </c>
       <c r="B98">
         <v>1235</v>
       </c>
+      <c r="C98">
+        <v>87</v>
+      </c>
       <c r="E98">
         <v>75</v>
       </c>
       <c r="F98">
         <v>1193</v>
       </c>
+      <c r="G98">
+        <v>174</v>
+      </c>
       <c r="I98">
         <v>80</v>
       </c>
       <c r="J98">
         <v>1051</v>
       </c>
+      <c r="K98">
+        <v>279</v>
+      </c>
       <c r="M98">
         <v>77</v>
       </c>
       <c r="N98">
         <v>1182</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O98">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -2911,360 +3974,522 @@
       <c r="F99">
         <v>1209</v>
       </c>
+      <c r="G99">
+        <v>175</v>
+      </c>
       <c r="I99">
         <v>81</v>
       </c>
       <c r="J99">
         <v>1057</v>
       </c>
+      <c r="K99">
+        <v>280</v>
+      </c>
       <c r="M99">
         <v>78</v>
       </c>
       <c r="N99">
         <v>1197</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O99">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
         <v>25</v>
       </c>
       <c r="F100">
         <v>1218</v>
       </c>
+      <c r="G100">
+        <v>176</v>
+      </c>
       <c r="I100">
         <v>82</v>
       </c>
       <c r="J100">
         <v>1061</v>
       </c>
+      <c r="K100">
+        <v>281</v>
+      </c>
       <c r="M100">
         <v>79</v>
       </c>
       <c r="N100">
         <v>1211</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O100">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E101" t="s">
         <v>26</v>
       </c>
       <c r="F101">
         <v>1221</v>
       </c>
+      <c r="G101">
+        <v>177</v>
+      </c>
       <c r="I101">
         <v>83</v>
       </c>
       <c r="J101">
         <v>1073</v>
       </c>
+      <c r="K101">
+        <v>282</v>
+      </c>
       <c r="M101">
         <v>80</v>
       </c>
       <c r="N101">
         <v>1221</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O101">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E102">
         <v>76</v>
       </c>
       <c r="F102">
         <v>1246</v>
       </c>
+      <c r="G102">
+        <v>178</v>
+      </c>
       <c r="I102">
         <v>84</v>
       </c>
       <c r="J102">
         <v>1091</v>
       </c>
+      <c r="K102">
+        <v>283</v>
+      </c>
       <c r="M102">
         <v>81</v>
       </c>
       <c r="N102">
         <v>1239</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O102">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E103">
         <v>77</v>
       </c>
       <c r="F103">
         <v>1265</v>
       </c>
+      <c r="G103">
+        <v>179</v>
+      </c>
       <c r="I103">
         <v>85</v>
       </c>
       <c r="J103">
         <v>1106</v>
       </c>
+      <c r="K103">
+        <v>284</v>
+      </c>
       <c r="M103">
         <v>82</v>
       </c>
       <c r="N103">
         <v>1246</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O103">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E104">
         <v>78</v>
       </c>
       <c r="F104">
         <v>1279</v>
       </c>
+      <c r="G104">
+        <v>180</v>
+      </c>
       <c r="I104">
         <v>86</v>
       </c>
       <c r="J104">
         <v>1110</v>
       </c>
+      <c r="K104">
+        <v>285</v>
+      </c>
       <c r="M104">
         <v>83</v>
       </c>
       <c r="N104">
         <v>1256</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O104">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E105">
         <v>79</v>
       </c>
       <c r="F105">
         <v>1291</v>
       </c>
+      <c r="G105">
+        <v>181</v>
+      </c>
       <c r="I105">
         <v>87</v>
       </c>
       <c r="J105">
         <v>1116</v>
       </c>
+      <c r="K105">
+        <v>286</v>
+      </c>
       <c r="M105">
         <v>84</v>
       </c>
       <c r="N105">
         <v>1270</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O105">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E106">
         <v>80</v>
       </c>
       <c r="F106">
         <v>1298</v>
       </c>
+      <c r="G106">
+        <v>182</v>
+      </c>
       <c r="I106" t="s">
         <v>16</v>
       </c>
       <c r="J106">
         <v>1121</v>
       </c>
+      <c r="K106">
+        <v>287</v>
+      </c>
       <c r="M106">
         <v>85</v>
       </c>
       <c r="N106">
         <v>1279</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O106">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E107">
         <v>81</v>
       </c>
       <c r="F107">
         <v>1310</v>
       </c>
+      <c r="G107">
+        <v>183</v>
+      </c>
       <c r="I107" t="s">
         <v>17</v>
       </c>
       <c r="J107">
         <v>1129</v>
       </c>
+      <c r="K107">
+        <v>288</v>
+      </c>
       <c r="M107">
         <v>86</v>
       </c>
       <c r="N107">
         <v>1287</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O107">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E108">
         <v>82</v>
       </c>
       <c r="F108">
         <v>1335</v>
       </c>
+      <c r="G108">
+        <v>184</v>
+      </c>
       <c r="I108" t="s">
         <v>18</v>
       </c>
       <c r="J108">
         <v>1133</v>
       </c>
+      <c r="K108">
+        <v>289</v>
+      </c>
       <c r="M108">
         <v>87</v>
       </c>
       <c r="N108">
         <v>1298</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O108">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E109">
         <v>83</v>
       </c>
       <c r="F109">
         <v>1351</v>
       </c>
+      <c r="G109">
+        <v>185</v>
+      </c>
       <c r="I109" t="s">
         <v>22</v>
       </c>
       <c r="J109">
         <v>1135</v>
       </c>
+      <c r="K109">
+        <v>290</v>
+      </c>
       <c r="M109">
         <v>88</v>
       </c>
       <c r="N109">
         <v>1316</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O109">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E110">
         <v>84</v>
       </c>
       <c r="F110">
         <v>1365</v>
       </c>
+      <c r="G110">
+        <v>186</v>
+      </c>
       <c r="I110" t="s">
         <v>23</v>
       </c>
       <c r="J110">
         <v>1139</v>
       </c>
+      <c r="K110">
+        <v>291</v>
+      </c>
       <c r="M110">
         <v>89</v>
       </c>
       <c r="N110">
         <v>1321</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O110">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E111">
         <v>85</v>
       </c>
       <c r="F111">
         <v>1377</v>
       </c>
+      <c r="G111">
+        <v>187</v>
+      </c>
       <c r="I111">
         <v>88</v>
       </c>
       <c r="J111">
         <v>1145</v>
       </c>
+      <c r="K111">
+        <v>292</v>
+      </c>
       <c r="M111">
         <v>90</v>
       </c>
       <c r="N111">
         <v>1331</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O111">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E112">
         <v>86</v>
       </c>
       <c r="F112">
         <v>1390</v>
       </c>
+      <c r="G112">
+        <v>188</v>
+      </c>
       <c r="I112">
         <v>89</v>
       </c>
       <c r="J112">
         <v>1154</v>
       </c>
+      <c r="K112">
+        <v>293</v>
+      </c>
       <c r="M112">
         <v>91</v>
       </c>
       <c r="N112">
         <v>1343</v>
       </c>
-    </row>
-    <row r="113" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O112">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="113" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E113">
         <v>87</v>
       </c>
       <c r="F113">
         <v>1412</v>
       </c>
+      <c r="G113">
+        <v>189</v>
+      </c>
       <c r="I113">
         <v>90</v>
       </c>
       <c r="J113">
         <v>1167</v>
       </c>
+      <c r="K113">
+        <v>294</v>
+      </c>
       <c r="M113">
         <v>92</v>
       </c>
       <c r="N113">
         <v>1352</v>
       </c>
-    </row>
-    <row r="114" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O113">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="114" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E114">
         <v>88</v>
       </c>
       <c r="F114">
         <v>1427</v>
       </c>
+      <c r="G114">
+        <v>190</v>
+      </c>
       <c r="I114">
         <v>91</v>
       </c>
       <c r="J114">
         <v>1174</v>
       </c>
+      <c r="K114">
+        <v>295</v>
+      </c>
       <c r="M114">
         <v>93</v>
       </c>
       <c r="N114">
         <v>1358</v>
       </c>
-    </row>
-    <row r="115" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O114">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="115" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E115">
         <v>89</v>
       </c>
       <c r="F115">
         <v>1442</v>
       </c>
+      <c r="G115">
+        <v>191</v>
+      </c>
       <c r="I115">
         <v>92</v>
       </c>
       <c r="J115">
         <v>1181</v>
       </c>
+      <c r="K115">
+        <v>296</v>
+      </c>
       <c r="M115">
         <v>94</v>
       </c>
       <c r="N115">
         <v>1371</v>
       </c>
-    </row>
-    <row r="116" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O115">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="116" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E116" t="s">
         <v>19</v>
       </c>
       <c r="F116">
         <v>1456</v>
       </c>
+      <c r="G116">
+        <v>192</v>
+      </c>
       <c r="I116">
         <v>93</v>
       </c>
       <c r="J116">
         <v>1193</v>
       </c>
+      <c r="K116">
+        <v>297</v>
+      </c>
       <c r="M116">
         <v>95</v>
       </c>
       <c r="N116">
         <v>1383</v>
       </c>
-    </row>
-    <row r="117" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O116">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="117" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E117" t="s">
         <v>20</v>
       </c>
@@ -3277,370 +4502,529 @@
       <c r="J117">
         <v>1201</v>
       </c>
+      <c r="K117">
+        <v>298</v>
+      </c>
       <c r="M117">
         <v>96</v>
       </c>
       <c r="N117">
         <v>1390</v>
       </c>
-    </row>
-    <row r="118" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O117">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="118" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I118">
         <v>95</v>
       </c>
       <c r="J118">
         <v>1205</v>
       </c>
+      <c r="K118">
+        <v>299</v>
+      </c>
       <c r="M118">
         <v>97</v>
       </c>
       <c r="N118">
         <v>1396</v>
       </c>
-    </row>
-    <row r="119" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O118">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="119" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I119">
         <v>96</v>
       </c>
       <c r="J119">
         <v>1211</v>
       </c>
+      <c r="K119">
+        <v>300</v>
+      </c>
       <c r="M119" t="s">
         <v>22</v>
       </c>
       <c r="N119">
         <v>1414</v>
       </c>
-    </row>
-    <row r="120" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O119">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="120" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I120">
         <v>97</v>
       </c>
       <c r="J120">
         <v>1226</v>
       </c>
+      <c r="K120">
+        <v>301</v>
+      </c>
       <c r="M120" t="s">
         <v>23</v>
       </c>
       <c r="N120">
         <v>1421</v>
       </c>
-    </row>
-    <row r="121" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O120">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="121" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I121">
         <v>98</v>
       </c>
       <c r="J121">
         <v>1241</v>
       </c>
+      <c r="K121">
+        <v>302</v>
+      </c>
       <c r="M121" t="s">
         <v>24</v>
       </c>
       <c r="N121">
         <v>1426</v>
       </c>
-    </row>
-    <row r="122" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O121">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="122" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I122">
         <v>99</v>
       </c>
       <c r="J122">
         <v>1251</v>
       </c>
+      <c r="K122">
+        <v>303</v>
+      </c>
       <c r="M122">
         <v>98</v>
       </c>
       <c r="N122">
         <v>1432</v>
       </c>
-    </row>
-    <row r="123" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O122">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="123" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I123">
         <v>100</v>
       </c>
       <c r="J123">
         <v>1264</v>
       </c>
+      <c r="K123">
+        <v>304</v>
+      </c>
       <c r="M123">
         <v>99</v>
       </c>
       <c r="N123">
         <v>1439</v>
       </c>
-    </row>
-    <row r="124" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O123">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="124" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I124">
         <v>101</v>
       </c>
       <c r="J124">
         <v>1277</v>
       </c>
+      <c r="K124">
+        <v>305</v>
+      </c>
       <c r="M124">
         <v>100</v>
       </c>
       <c r="N124">
         <v>1448</v>
       </c>
-    </row>
-    <row r="125" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O124">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="125" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I125">
         <v>102</v>
       </c>
       <c r="J125">
         <v>1286</v>
       </c>
+      <c r="K125">
+        <v>306</v>
+      </c>
       <c r="M125">
         <v>101</v>
       </c>
       <c r="N125">
         <v>1453</v>
       </c>
-    </row>
-    <row r="126" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O125">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="126" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I126">
         <v>103</v>
       </c>
       <c r="J126">
         <v>1302</v>
       </c>
+      <c r="K126">
+        <v>307</v>
+      </c>
       <c r="M126">
         <v>102</v>
       </c>
       <c r="N126">
         <v>1466</v>
       </c>
-    </row>
-    <row r="127" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O126">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="127" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I127">
         <v>104</v>
       </c>
       <c r="J127">
         <v>1313</v>
       </c>
+      <c r="K127">
+        <v>308</v>
+      </c>
       <c r="M127">
         <v>103</v>
       </c>
       <c r="N127">
         <v>1479</v>
       </c>
-    </row>
-    <row r="128" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="O127">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="128" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I128">
         <v>105</v>
       </c>
       <c r="J128">
         <v>1323</v>
       </c>
+      <c r="K128">
+        <v>309</v>
+      </c>
       <c r="M128">
         <v>104</v>
       </c>
       <c r="N128">
         <v>1486</v>
       </c>
-    </row>
-    <row r="129" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O128">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="129" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I129">
         <v>106</v>
       </c>
       <c r="J129">
         <v>1333</v>
       </c>
+      <c r="K129">
+        <v>310</v>
+      </c>
       <c r="M129">
         <v>105</v>
       </c>
       <c r="N129">
         <v>1495</v>
       </c>
-    </row>
-    <row r="130" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O129">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="130" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I130">
         <v>107</v>
       </c>
       <c r="J130">
         <v>1340</v>
       </c>
+      <c r="K130">
+        <v>311</v>
+      </c>
       <c r="M130">
         <v>106</v>
       </c>
       <c r="N130">
         <v>1503</v>
       </c>
-    </row>
-    <row r="131" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O130">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="131" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I131">
         <v>108</v>
       </c>
       <c r="J131">
         <v>1362</v>
       </c>
+      <c r="K131">
+        <v>312</v>
+      </c>
       <c r="M131">
         <v>107</v>
       </c>
       <c r="N131">
         <v>1512</v>
       </c>
-    </row>
-    <row r="132" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O131">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="132" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I132">
         <v>109</v>
       </c>
       <c r="J132">
         <v>1382</v>
       </c>
+      <c r="K132">
+        <v>313</v>
+      </c>
       <c r="M132">
         <v>108</v>
       </c>
       <c r="N132">
         <v>1519</v>
       </c>
-    </row>
-    <row r="133" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O132">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="133" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I133">
         <v>110</v>
       </c>
       <c r="J133">
         <v>1396</v>
       </c>
+      <c r="K133">
+        <v>314</v>
+      </c>
       <c r="M133">
         <v>109</v>
       </c>
       <c r="N133">
         <v>1525</v>
       </c>
-    </row>
-    <row r="134" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O133">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="134" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I134">
         <v>111</v>
       </c>
       <c r="J134">
         <v>1403</v>
       </c>
+      <c r="K134">
+        <v>315</v>
+      </c>
       <c r="M134">
         <v>110</v>
       </c>
       <c r="N134">
         <v>1533</v>
       </c>
-    </row>
-    <row r="135" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O134">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="135" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I135">
         <v>112</v>
       </c>
       <c r="J135">
         <v>1418</v>
       </c>
+      <c r="K135">
+        <v>316</v>
+      </c>
       <c r="M135">
         <v>111</v>
       </c>
       <c r="N135">
         <v>1539</v>
       </c>
-    </row>
-    <row r="136" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O135">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="136" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I136">
         <v>113</v>
       </c>
       <c r="J136">
         <v>1423</v>
       </c>
+      <c r="K136">
+        <v>317</v>
+      </c>
       <c r="M136">
         <v>112</v>
       </c>
       <c r="N136">
         <v>1565</v>
       </c>
-    </row>
-    <row r="137" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O136">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="137" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I137" t="s">
         <v>24</v>
       </c>
       <c r="J137">
         <v>1431</v>
       </c>
+      <c r="K137">
+        <v>318</v>
+      </c>
       <c r="M137">
         <v>113</v>
       </c>
       <c r="N137">
         <v>1577</v>
       </c>
-    </row>
-    <row r="138" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O137">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="138" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I138" t="s">
         <v>25</v>
       </c>
       <c r="J138">
         <v>1434</v>
       </c>
+      <c r="K138">
+        <v>319</v>
+      </c>
       <c r="M138">
         <v>114</v>
       </c>
       <c r="N138">
         <v>1587</v>
       </c>
-    </row>
-    <row r="139" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O138">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="139" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I139" t="s">
         <v>26</v>
       </c>
       <c r="J139">
         <v>1448</v>
       </c>
+      <c r="K139">
+        <v>320</v>
+      </c>
       <c r="M139">
         <v>115</v>
       </c>
       <c r="N139">
         <v>1595</v>
       </c>
-    </row>
-    <row r="140" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O139">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="140" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I140">
         <v>114</v>
       </c>
       <c r="J140">
         <v>1452</v>
       </c>
+      <c r="K140">
+        <v>321</v>
+      </c>
       <c r="M140">
         <v>116</v>
       </c>
       <c r="N140">
         <v>1604</v>
       </c>
-    </row>
-    <row r="141" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O140">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="141" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I141">
         <v>115</v>
       </c>
       <c r="J141">
         <v>1464</v>
       </c>
+      <c r="K141">
+        <v>322</v>
+      </c>
       <c r="M141">
         <v>117</v>
       </c>
       <c r="N141">
         <v>1614</v>
       </c>
-    </row>
-    <row r="142" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O141">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="142" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I142">
         <v>116</v>
       </c>
       <c r="J142">
         <v>1480</v>
       </c>
+      <c r="K142">
+        <v>323</v>
+      </c>
       <c r="M142" t="s">
         <v>19</v>
       </c>
       <c r="N142">
         <v>1621</v>
       </c>
-    </row>
-    <row r="143" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="O142">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="143" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I143">
         <v>117</v>
       </c>
       <c r="J143">
         <v>1499</v>
       </c>
+      <c r="K143">
+        <v>324</v>
+      </c>
       <c r="M143" t="s">
         <v>20</v>
       </c>
@@ -3648,55 +5032,73 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="144" spans="9:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I144">
         <v>118</v>
       </c>
       <c r="J144">
         <v>1519</v>
       </c>
-    </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K144">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="145" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I145">
         <v>119</v>
       </c>
       <c r="J145">
         <v>1533</v>
       </c>
-    </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K145">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="146" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I146">
         <v>120</v>
       </c>
       <c r="J146">
         <v>1547</v>
       </c>
-    </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K146">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="147" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I147">
         <v>121</v>
       </c>
       <c r="J147">
         <v>1608</v>
       </c>
-    </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K147">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="148" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I148">
         <v>122</v>
       </c>
       <c r="J148">
         <v>1637</v>
       </c>
-    </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K148">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="149" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I149" t="s">
         <v>19</v>
       </c>
       <c r="J149">
         <v>1662</v>
       </c>
-    </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="K149">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="150" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I150" t="s">
         <v>20</v>
       </c>

</xml_diff>